<commit_message>
Solve mass balance trouble when pump is turning on
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{CF18C2C8-D5B4-4E78-AA05-D0055054A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8228064B-094D-4872-B154-FB73C4AF3BB5}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{CF18C2C8-D5B4-4E78-AA05-D0055054A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A89F6790-9B26-46AA-8D07-510A14607BAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="669">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -2076,6 +2076,12 @@
   </si>
   <si>
     <t>SV-109</t>
+  </si>
+  <si>
+    <t>concentración de dolidos volátiles a la salida del reactor 1</t>
+  </si>
+  <si>
+    <t>concentracion de sólidos totales a la salida del reactor 1</t>
   </si>
 </sst>
 </file>
@@ -6562,10 +6568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7691,13 +7697,36 @@
         <v>625</v>
       </c>
       <c r="B102" t="s">
+        <v>667</v>
+      </c>
+      <c r="C102" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>625</v>
+      </c>
+      <c r="B103" t="s">
+        <v>668</v>
+      </c>
+      <c r="C103" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>625</v>
+      </c>
+      <c r="B104" t="s">
         <v>644</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C104" t="s">
         <v>645</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Biogas storage model updating
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{CF18C2C8-D5B4-4E78-AA05-D0055054A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A89F6790-9B26-46AA-8D07-510A14607BAD}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{CF18C2C8-D5B4-4E78-AA05-D0055054A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9333A0F-28DD-421E-8748-4CEED7A8286F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="677">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -1967,18 +1967,9 @@
     <t>TE-101v</t>
   </si>
   <si>
-    <t>Volumen normal de biogás (almacenadas)</t>
-  </si>
-  <si>
     <t>M-VGA</t>
   </si>
   <si>
-    <t>Volumen parcial  metano (almacenadas)</t>
-  </si>
-  <si>
-    <t>M-PA_CH4</t>
-  </si>
-  <si>
     <t>moles metano (almacenadas)</t>
   </si>
   <si>
@@ -2082,6 +2073,39 @@
   </si>
   <si>
     <t>concentracion de sólidos totales a la salida del reactor 1</t>
+  </si>
+  <si>
+    <t>Volumen normal de biogás (almacenadas) V-101</t>
+  </si>
+  <si>
+    <t>Volumen parcial  metano (almacenadas) V-101</t>
+  </si>
+  <si>
+    <t>Volumen parcial de dióxido de carbono (almacenadas) V-101</t>
+  </si>
+  <si>
+    <t>M-PA_CH4_1</t>
+  </si>
+  <si>
+    <t>M-PA_CO2_1</t>
+  </si>
+  <si>
+    <t>M-PA_H2S_1</t>
+  </si>
+  <si>
+    <t>Volumen parcial de Sulfuro de hidrógeno (almacenadas) V-101</t>
+  </si>
+  <si>
+    <t>Volumen parcial de oxigeno (almacenadas) V-101</t>
+  </si>
+  <si>
+    <t>M-PA_O2_1</t>
+  </si>
+  <si>
+    <t>Volumen Parcial de hidrógeno (almacenadas) V-101</t>
+  </si>
+  <si>
+    <t>M-PA_H2_1</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2148,6 +2172,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2164,7 +2194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2177,6 +2207,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2567,7 +2598,7 @@
         <v>440</v>
       </c>
       <c r="E5" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F5" t="s">
         <v>527</v>
@@ -6568,10 +6599,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7466,10 +7497,10 @@
         <v>528</v>
       </c>
       <c r="B81" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C81" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -7477,10 +7508,10 @@
         <v>528</v>
       </c>
       <c r="B82" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C82" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -7488,7 +7519,7 @@
         <v>528</v>
       </c>
       <c r="B83" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C83" t="s">
         <v>574</v>
@@ -7499,10 +7530,10 @@
         <v>528</v>
       </c>
       <c r="B84" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C84" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -7510,10 +7541,10 @@
         <v>528</v>
       </c>
       <c r="B85" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C85" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -7521,10 +7552,10 @@
         <v>528</v>
       </c>
       <c r="B86" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C86" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -7543,10 +7574,10 @@
         <v>528</v>
       </c>
       <c r="B88" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C88" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -7554,10 +7585,10 @@
         <v>528</v>
       </c>
       <c r="B89" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C89" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -7565,10 +7596,10 @@
         <v>528</v>
       </c>
       <c r="B90" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C90" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -7576,10 +7607,10 @@
         <v>528</v>
       </c>
       <c r="B91" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C91" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -7587,10 +7618,10 @@
         <v>528</v>
       </c>
       <c r="B92" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C92" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -7620,10 +7651,10 @@
         <v>625</v>
       </c>
       <c r="B95" t="s">
+        <v>666</v>
+      </c>
+      <c r="C95" t="s">
         <v>630</v>
-      </c>
-      <c r="C95" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -7631,10 +7662,10 @@
         <v>625</v>
       </c>
       <c r="B96" t="s">
-        <v>632</v>
+        <v>667</v>
       </c>
       <c r="C96" t="s">
-        <v>633</v>
+        <v>669</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -7642,10 +7673,10 @@
         <v>625</v>
       </c>
       <c r="B97" t="s">
-        <v>634</v>
+        <v>668</v>
       </c>
       <c r="C97" t="s">
-        <v>635</v>
+        <v>670</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -7653,10 +7684,10 @@
         <v>625</v>
       </c>
       <c r="B98" t="s">
-        <v>636</v>
+        <v>672</v>
       </c>
       <c r="C98" t="s">
-        <v>637</v>
+        <v>671</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -7664,21 +7695,21 @@
         <v>625</v>
       </c>
       <c r="B99" t="s">
-        <v>638</v>
+        <v>673</v>
       </c>
       <c r="C99" t="s">
-        <v>639</v>
+        <v>674</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="B100" t="s">
-        <v>640</v>
-      </c>
-      <c r="C100" t="s">
-        <v>641</v>
+      <c r="B100" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -7686,10 +7717,10 @@
         <v>625</v>
       </c>
       <c r="B101" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="C101" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -7697,10 +7728,10 @@
         <v>625</v>
       </c>
       <c r="B102" t="s">
-        <v>667</v>
+        <v>633</v>
       </c>
       <c r="C102" t="s">
-        <v>552</v>
+        <v>634</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -7708,10 +7739,10 @@
         <v>625</v>
       </c>
       <c r="B103" t="s">
-        <v>668</v>
+        <v>635</v>
       </c>
       <c r="C103" t="s">
-        <v>550</v>
+        <v>636</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -7719,10 +7750,54 @@
         <v>625</v>
       </c>
       <c r="B104" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="C104" t="s">
-        <v>645</v>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>625</v>
+      </c>
+      <c r="B105" t="s">
+        <v>639</v>
+      </c>
+      <c r="C105" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>625</v>
+      </c>
+      <c r="B106" t="s">
+        <v>664</v>
+      </c>
+      <c r="C106" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>625</v>
+      </c>
+      <c r="B107" t="s">
+        <v>665</v>
+      </c>
+      <c r="C107" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>625</v>
+      </c>
+      <c r="B108" t="s">
+        <v>641</v>
+      </c>
+      <c r="C108" t="s">
+        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solar model backend implementation
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\backend\v1.0\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{CF18C2C8-D5B4-4E78-AA05-D0055054A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE0ADA7C-2946-42CC-8602-052FE9D900B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621441D7-9BB4-465E-80DF-51E0AC2CF6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="721">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -1967,9 +1967,18 @@
     <t>TE-101v</t>
   </si>
   <si>
+    <t>Volumen normal de biogás (almacenadas)</t>
+  </si>
+  <si>
     <t>M-VGA</t>
   </si>
   <si>
+    <t>Volumen parcial  metano (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_CH4</t>
+  </si>
+  <si>
     <t>moles metano (almacenadas)</t>
   </si>
   <si>
@@ -2075,44 +2084,167 @@
     <t>concentracion de sólidos totales a la salida del reactor 1</t>
   </si>
   <si>
-    <t>Volumen normal de biogás (almacenadas) V-101</t>
-  </si>
-  <si>
-    <t>Volumen parcial  metano (almacenadas) V-101</t>
-  </si>
-  <si>
-    <t>Volumen parcial de dióxido de carbono (almacenadas) V-101</t>
-  </si>
-  <si>
-    <t>M-PA_CH4_1</t>
-  </si>
-  <si>
-    <t>M-PA_CO2_1</t>
-  </si>
-  <si>
-    <t>M-PA_H2S_1</t>
-  </si>
-  <si>
-    <t>Volumen parcial de Sulfuro de hidrógeno (almacenadas) V-101</t>
-  </si>
-  <si>
-    <t>Volumen parcial de oxigeno (almacenadas) V-101</t>
-  </si>
-  <si>
-    <t>M-PA_O2_1</t>
-  </si>
-  <si>
-    <t>Volumen Parcial de hidrógeno (almacenadas) V-101</t>
-  </si>
-  <si>
-    <t>M-PA_H2_1</t>
+    <t>Módulo solar-eólico</t>
+  </si>
+  <si>
+    <t>Radiación paneles solares 1 (pv)</t>
+  </si>
+  <si>
+    <t>RS001</t>
+  </si>
+  <si>
+    <t>Radiación paneles solares 2 (pv)</t>
+  </si>
+  <si>
+    <t>RS002</t>
+  </si>
+  <si>
+    <t>Velocidad de viento aerogenerador (fan)</t>
+  </si>
+  <si>
+    <t>VV001</t>
+  </si>
+  <si>
+    <t>RPMs aerogenerador (fan)</t>
+  </si>
+  <si>
+    <t>RPM001</t>
+  </si>
+  <si>
+    <t>Temperatura para los 4 Paneles (pv)</t>
+  </si>
+  <si>
+    <t>TE004</t>
+  </si>
+  <si>
+    <t>Voltaje Paneles solares (pv)  (Controlador)</t>
+  </si>
+  <si>
+    <t>Corriente paneles  (pv) (Controlador)</t>
+  </si>
+  <si>
+    <t>Potencia paneles (pv) (Controlador)</t>
+  </si>
+  <si>
+    <t>Voltaje aerogenerador (fan) (Controlador)</t>
+  </si>
+  <si>
+    <t>VG005</t>
+  </si>
+  <si>
+    <t>Corriente Aerogenerador (fan) (Controlador)</t>
+  </si>
+  <si>
+    <t>IG005</t>
+  </si>
+  <si>
+    <t>Potencia aerogenerador (fan)(Controlador)</t>
+  </si>
+  <si>
+    <t>PG005</t>
+  </si>
+  <si>
+    <t>Voltaje de las baterías (Controlador)</t>
+  </si>
+  <si>
+    <t>Energía generada por paneles (kWh) (pv) (Controlador)</t>
+  </si>
+  <si>
+    <t>Energía generada por aerogenerador (kWh)(fan) (Controlador)</t>
+  </si>
+  <si>
+    <t>EG002</t>
+  </si>
+  <si>
+    <t>Voltaje bulk controlador de carga</t>
+  </si>
+  <si>
+    <t>Voltaje float controlador de carga</t>
+  </si>
+  <si>
+    <t>Voltaje de carga controlador de carga</t>
+  </si>
+  <si>
+    <t>Potencia aparente salida del inversor (inversor o analizador)</t>
+  </si>
+  <si>
+    <t>Potencia Reactiva salida del inversor (analizador)</t>
+  </si>
+  <si>
+    <t>Factor de Potencia salida del inversor (analizador)</t>
+  </si>
+  <si>
+    <t>Potencia activa salida del inversor (analizador)</t>
+  </si>
+  <si>
+    <t>Voltaje AC a la salida del inversor hibrido (inversor o analizador)</t>
+  </si>
+  <si>
+    <t>VAC002</t>
+  </si>
+  <si>
+    <t>Corriente a la salida del inversor hibrido (inversor o analizador)</t>
+  </si>
+  <si>
+    <t>IAC002</t>
+  </si>
+  <si>
+    <t>Potencia aparente salida del inversor hibrido (inversor o analizador)</t>
+  </si>
+  <si>
+    <t>PKVA002</t>
+  </si>
+  <si>
+    <t>Potencia Reactiva salida del inversor hibrido (analizador)</t>
+  </si>
+  <si>
+    <t>PKVAR002</t>
+  </si>
+  <si>
+    <t>Factor de Potencia salida del inversor hibrido (analizador)</t>
+  </si>
+  <si>
+    <t>FP002</t>
+  </si>
+  <si>
+    <t>Potencia activa salida del inversor hibrido (analizador)</t>
+  </si>
+  <si>
+    <t>PKW002</t>
+  </si>
+  <si>
+    <t>Voltaje bulk inversor hibrido</t>
+  </si>
+  <si>
+    <t>VBU002</t>
+  </si>
+  <si>
+    <t>Voltaje float inversor hibrido</t>
+  </si>
+  <si>
+    <t>VFL002</t>
+  </si>
+  <si>
+    <t>Voltaje de carga inversor hibrido</t>
+  </si>
+  <si>
+    <t>VCH002</t>
+  </si>
+  <si>
+    <t>Estado del inversor aislado</t>
+  </si>
+  <si>
+    <t>Estado de la red inversor hibrido</t>
+  </si>
+  <si>
+    <t>ER001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2162,7 +2294,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2172,12 +2304,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2194,7 +2320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2207,7 +2333,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2223,10 +2348,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2498,13 +2619,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>275</v>
       </c>
@@ -2524,7 +2645,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>436</v>
       </c>
@@ -2544,7 +2665,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>436</v>
       </c>
@@ -2564,7 +2685,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>525</v>
       </c>
@@ -2584,7 +2705,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>436</v>
       </c>
@@ -2598,13 +2719,13 @@
         <v>440</v>
       </c>
       <c r="E5" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="F5" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="E10" s="8"/>
     </row>
   </sheetData>
@@ -2621,13 +2742,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>275</v>
       </c>
@@ -2641,7 +2762,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>435</v>
       </c>
@@ -2665,17 +2786,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>428</v>
       </c>
@@ -2686,7 +2807,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2697,7 +2818,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2708,7 +2829,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2719,7 +2840,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2730,7 +2851,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2741,7 +2862,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2752,7 +2873,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2763,7 +2884,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2774,7 +2895,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2785,7 +2906,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2796,7 +2917,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2807,7 +2928,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2818,7 +2939,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2829,7 +2950,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2840,7 +2961,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2851,7 +2972,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2862,7 +2983,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2873,7 +2994,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2884,7 +3005,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2895,7 +3016,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2906,136 +3027,136 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1">
       <c r="A55" s="6"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1">
       <c r="A56" s="6"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1">
       <c r="A57" s="6"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1">
       <c r="A58" s="6"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1">
       <c r="A61" s="6"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1">
       <c r="A62" s="6"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1">
       <c r="A63" s="6"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1">
       <c r="A64" s="6"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1">
       <c r="A65" s="6"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1">
       <c r="A66" s="6"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1">
       <c r="A67" s="6"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1">
       <c r="A68" s="6"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1">
       <c r="A69" s="6"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1">
       <c r="A70" s="6"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1">
       <c r="A71" s="6"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1">
       <c r="A72" s="6"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1">
       <c r="A73" s="6"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1">
       <c r="A74" s="6"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1">
       <c r="A75" s="6"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1">
       <c r="A76" s="6"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1">
       <c r="A77" s="6"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1">
       <c r="A78" s="6"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1">
       <c r="A79" s="6"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1">
       <c r="A80" s="6"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1">
       <c r="A93" s="2"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1">
       <c r="A115" s="6"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1">
       <c r="A116" s="6"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1">
       <c r="A117" s="6"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1">
       <c r="A118" s="6"/>
     </row>
   </sheetData>
@@ -3051,18 +3172,18 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -3088,7 +3209,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3114,7 +3235,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3140,7 +3261,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3166,7 +3287,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3192,7 +3313,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3218,7 +3339,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3244,7 +3365,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3270,7 +3391,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3296,7 +3417,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3322,7 +3443,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3348,7 +3469,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3374,7 +3495,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3400,7 +3521,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -3426,7 +3547,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -3452,7 +3573,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -3478,7 +3599,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -3504,7 +3625,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3530,7 +3651,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -3556,7 +3677,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3579,7 +3700,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3602,7 +3723,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3625,7 +3746,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3651,7 +3772,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3677,7 +3798,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3703,7 +3824,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3729,7 +3850,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3755,7 +3876,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3781,7 +3902,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3807,7 +3928,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -3833,7 +3954,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -3859,7 +3980,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3885,7 +4006,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -3911,7 +4032,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -3937,7 +4058,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -3963,7 +4084,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -3989,7 +4110,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -4015,7 +4136,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -4041,7 +4162,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -4067,7 +4188,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -4093,7 +4214,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -4119,7 +4240,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -4145,7 +4266,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -4171,7 +4292,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -4197,7 +4318,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -4223,7 +4344,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>211</v>
       </c>
@@ -4249,7 +4370,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>212</v>
       </c>
@@ -4275,7 +4396,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>213</v>
       </c>
@@ -4301,7 +4422,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>214</v>
       </c>
@@ -4327,7 +4448,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>215</v>
       </c>
@@ -4353,7 +4474,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -4379,7 +4500,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>217</v>
       </c>
@@ -4405,7 +4526,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>218</v>
       </c>
@@ -4431,7 +4552,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>219</v>
       </c>
@@ -4457,7 +4578,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>220</v>
       </c>
@@ -4483,7 +4604,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -4509,7 +4630,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -4535,7 +4656,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -4561,7 +4682,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -4587,7 +4708,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>223</v>
       </c>
@@ -4613,7 +4734,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>224</v>
       </c>
@@ -4639,7 +4760,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -4665,7 +4786,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>226</v>
       </c>
@@ -4691,7 +4812,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>227</v>
       </c>
@@ -4717,7 +4838,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>228</v>
       </c>
@@ -4743,7 +4864,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4769,7 +4890,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>230</v>
       </c>
@@ -4795,7 +4916,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -4821,7 +4942,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -4847,7 +4968,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>233</v>
       </c>
@@ -4873,7 +4994,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -4899,7 +5020,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -4925,7 +5046,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -4951,7 +5072,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>235</v>
       </c>
@@ -4977,7 +5098,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>236</v>
       </c>
@@ -5003,7 +5124,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>237</v>
       </c>
@@ -5029,7 +5150,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>238</v>
       </c>
@@ -5055,7 +5176,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -5081,7 +5202,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>240</v>
       </c>
@@ -5107,7 +5228,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -5133,7 +5254,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>242</v>
       </c>
@@ -5159,7 +5280,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>243</v>
       </c>
@@ -5185,7 +5306,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>244</v>
       </c>
@@ -5211,7 +5332,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>245</v>
       </c>
@@ -5237,7 +5358,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>246</v>
       </c>
@@ -5263,7 +5384,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>247</v>
       </c>
@@ -5289,7 +5410,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>116</v>
       </c>
@@ -5315,7 +5436,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>118</v>
       </c>
@@ -5341,7 +5462,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>248</v>
       </c>
@@ -5367,7 +5488,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>249</v>
       </c>
@@ -5393,7 +5514,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>250</v>
       </c>
@@ -5419,7 +5540,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -5445,7 +5566,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>252</v>
       </c>
@@ -5471,7 +5592,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>253</v>
       </c>
@@ -5497,7 +5618,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>254</v>
       </c>
@@ -5523,7 +5644,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>255</v>
       </c>
@@ -5549,7 +5670,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>256</v>
       </c>
@@ -5575,7 +5696,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>257</v>
       </c>
@@ -5601,7 +5722,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>258</v>
       </c>
@@ -5627,7 +5748,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>259</v>
       </c>
@@ -5653,7 +5774,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>260</v>
       </c>
@@ -5679,7 +5800,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -5705,7 +5826,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -5731,7 +5852,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>261</v>
       </c>
@@ -5757,7 +5878,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>262</v>
       </c>
@@ -5783,7 +5904,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>263</v>
       </c>
@@ -5809,7 +5930,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>264</v>
       </c>
@@ -5835,7 +5956,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>265</v>
       </c>
@@ -5861,7 +5982,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>266</v>
       </c>
@@ -5887,7 +6008,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>267</v>
       </c>
@@ -5913,7 +6034,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>268</v>
       </c>
@@ -5939,7 +6060,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>269</v>
       </c>
@@ -5965,7 +6086,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>270</v>
       </c>
@@ -5991,7 +6112,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>271</v>
       </c>
@@ -6017,7 +6138,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>272</v>
       </c>
@@ -6043,7 +6164,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>273</v>
       </c>
@@ -6069,7 +6190,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>60</v>
       </c>
@@ -6095,7 +6216,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>62</v>
       </c>
@@ -6121,7 +6242,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>64</v>
       </c>
@@ -6147,7 +6268,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>66</v>
       </c>
@@ -6173,7 +6294,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -6199,7 +6320,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>70</v>
       </c>
@@ -6225,7 +6346,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -6251,7 +6372,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>74</v>
       </c>
@@ -6277,7 +6398,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>76</v>
       </c>
@@ -6303,7 +6424,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>78</v>
       </c>
@@ -6329,7 +6450,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>80</v>
       </c>
@@ -6355,7 +6476,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>82</v>
       </c>
@@ -6381,7 +6502,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>84</v>
       </c>
@@ -6407,7 +6528,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>86</v>
       </c>
@@ -6433,7 +6554,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8">
       <c r="A131" s="6" t="s">
         <v>88</v>
       </c>
@@ -6459,7 +6580,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8">
       <c r="A132" s="6" t="s">
         <v>90</v>
       </c>
@@ -6485,7 +6606,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8">
       <c r="A133" s="6" t="s">
         <v>92</v>
       </c>
@@ -6511,7 +6632,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8">
       <c r="A134" s="6" t="s">
         <v>94</v>
       </c>
@@ -6537,7 +6658,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>96</v>
       </c>
@@ -6563,7 +6684,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>98</v>
       </c>
@@ -6599,20 +6720,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>465</v>
       </c>
@@ -6623,7 +6744,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -6634,7 +6755,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -6645,7 +6766,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>467</v>
       </c>
@@ -6656,7 +6777,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>467</v>
       </c>
@@ -6667,7 +6788,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>467</v>
       </c>
@@ -6678,7 +6799,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>467</v>
       </c>
@@ -6689,7 +6810,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>467</v>
       </c>
@@ -6700,7 +6821,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -6711,7 +6832,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>467</v>
       </c>
@@ -6722,7 +6843,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>467</v>
       </c>
@@ -6733,7 +6854,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>467</v>
       </c>
@@ -6744,7 +6865,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>467</v>
       </c>
@@ -6755,7 +6876,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>467</v>
       </c>
@@ -6766,7 +6887,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>467</v>
       </c>
@@ -6777,7 +6898,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>467</v>
       </c>
@@ -6788,7 +6909,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>467</v>
       </c>
@@ -6799,7 +6920,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>467</v>
       </c>
@@ -6810,7 +6931,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>467</v>
       </c>
@@ -6821,7 +6942,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>467</v>
       </c>
@@ -6832,7 +6953,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>467</v>
       </c>
@@ -6843,7 +6964,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>467</v>
       </c>
@@ -6854,7 +6975,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>467</v>
       </c>
@@ -6865,7 +6986,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="9" t="s">
         <v>467</v>
       </c>
@@ -6876,7 +6997,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="9" t="s">
         <v>467</v>
       </c>
@@ -6887,7 +7008,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="9" t="s">
         <v>467</v>
       </c>
@@ -6898,7 +7019,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="9" t="s">
         <v>467</v>
       </c>
@@ -6909,7 +7030,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="9" t="s">
         <v>467</v>
       </c>
@@ -6920,7 +7041,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="9" t="s">
         <v>467</v>
       </c>
@@ -6931,7 +7052,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="9" t="s">
         <v>467</v>
       </c>
@@ -6942,7 +7063,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="9" t="s">
         <v>467</v>
       </c>
@@ -6953,7 +7074,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>528</v>
       </c>
@@ -6964,7 +7085,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>528</v>
       </c>
@@ -6975,7 +7096,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>528</v>
       </c>
@@ -6986,7 +7107,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>528</v>
       </c>
@@ -6997,7 +7118,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>528</v>
       </c>
@@ -7008,7 +7129,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>528</v>
       </c>
@@ -7019,7 +7140,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>528</v>
       </c>
@@ -7030,7 +7151,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>528</v>
       </c>
@@ -7041,7 +7162,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>528</v>
       </c>
@@ -7052,7 +7173,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>528</v>
       </c>
@@ -7063,7 +7184,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>528</v>
       </c>
@@ -7074,7 +7195,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>528</v>
       </c>
@@ -7085,7 +7206,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>528</v>
       </c>
@@ -7096,7 +7217,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>528</v>
       </c>
@@ -7107,7 +7228,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>528</v>
       </c>
@@ -7118,7 +7239,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>528</v>
       </c>
@@ -7129,7 +7250,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>528</v>
       </c>
@@ -7140,7 +7261,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>528</v>
       </c>
@@ -7151,7 +7272,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>528</v>
       </c>
@@ -7162,7 +7283,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>528</v>
       </c>
@@ -7173,7 +7294,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>528</v>
       </c>
@@ -7184,7 +7305,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>528</v>
       </c>
@@ -7195,7 +7316,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>528</v>
       </c>
@@ -7206,7 +7327,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>528</v>
       </c>
@@ -7217,7 +7338,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>528</v>
       </c>
@@ -7228,7 +7349,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>528</v>
       </c>
@@ -7239,7 +7360,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>528</v>
       </c>
@@ -7250,7 +7371,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>528</v>
       </c>
@@ -7261,7 +7382,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>528</v>
       </c>
@@ -7272,7 +7393,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>528</v>
       </c>
@@ -7283,7 +7404,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>528</v>
       </c>
@@ -7294,7 +7415,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>528</v>
       </c>
@@ -7305,7 +7426,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>528</v>
       </c>
@@ -7316,7 +7437,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>528</v>
       </c>
@@ -7327,7 +7448,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>528</v>
       </c>
@@ -7338,7 +7459,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>528</v>
       </c>
@@ -7349,7 +7470,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>528</v>
       </c>
@@ -7360,7 +7481,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>528</v>
       </c>
@@ -7371,7 +7492,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>528</v>
       </c>
@@ -7382,7 +7503,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>528</v>
       </c>
@@ -7393,7 +7514,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>528</v>
       </c>
@@ -7404,7 +7525,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>528</v>
       </c>
@@ -7415,7 +7536,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>528</v>
       </c>
@@ -7426,7 +7547,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>528</v>
       </c>
@@ -7437,7 +7558,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>528</v>
       </c>
@@ -7448,7 +7569,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>528</v>
       </c>
@@ -7459,7 +7580,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>528</v>
       </c>
@@ -7470,7 +7591,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>528</v>
       </c>
@@ -7481,7 +7602,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>528</v>
       </c>
@@ -7492,73 +7613,73 @@
         <v>624</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>528</v>
       </c>
       <c r="B81" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="C81" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>528</v>
       </c>
       <c r="B82" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="C82" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>528</v>
       </c>
       <c r="B83" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="C83" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>528</v>
       </c>
       <c r="B84" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="C84" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>528</v>
       </c>
       <c r="B85" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C85" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>528</v>
       </c>
       <c r="B86" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C86" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>528</v>
       </c>
@@ -7569,62 +7690,62 @@
         <v>600</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>528</v>
       </c>
       <c r="B88" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="C88" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>528</v>
       </c>
       <c r="B89" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C89" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>528</v>
       </c>
       <c r="B90" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="C90" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>528</v>
       </c>
       <c r="B91" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C91" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>528</v>
       </c>
       <c r="B92" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="C92" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>625</v>
       </c>
@@ -7635,7 +7756,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>625</v>
       </c>
@@ -7646,164 +7767,521 @@
         <v>629</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>625</v>
       </c>
       <c r="B95" t="s">
-        <v>666</v>
+        <v>630</v>
       </c>
       <c r="C95" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>625</v>
       </c>
       <c r="B96" t="s">
-        <v>667</v>
+        <v>632</v>
       </c>
       <c r="C96" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>625</v>
       </c>
       <c r="B97" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
       <c r="C97" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>625</v>
       </c>
       <c r="B98" t="s">
-        <v>672</v>
+        <v>636</v>
       </c>
       <c r="C98" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>625</v>
       </c>
       <c r="B99" t="s">
-        <v>673</v>
+        <v>638</v>
       </c>
       <c r="C99" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
         <v>625</v>
       </c>
-      <c r="B100" s="10" t="s">
-        <v>675</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>640</v>
+      </c>
+      <c r="C100" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>625</v>
       </c>
       <c r="B101" t="s">
-        <v>631</v>
+        <v>642</v>
       </c>
       <c r="C101" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>625</v>
       </c>
-      <c r="B102" s="8"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>667</v>
+      </c>
+      <c r="C102" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>625</v>
       </c>
       <c r="B103" t="s">
-        <v>633</v>
+        <v>668</v>
       </c>
       <c r="C103" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>625</v>
       </c>
       <c r="B104" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="C104" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>625</v>
+        <v>669</v>
       </c>
       <c r="B105" t="s">
-        <v>637</v>
+        <v>670</v>
       </c>
       <c r="C105" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>625</v>
+        <v>669</v>
       </c>
       <c r="B106" t="s">
-        <v>639</v>
+        <v>672</v>
       </c>
       <c r="C106" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>625</v>
+        <v>669</v>
       </c>
       <c r="B107" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="C107" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>625</v>
+        <v>669</v>
       </c>
       <c r="B108" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="C108" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>625</v>
+        <v>669</v>
       </c>
       <c r="B109" t="s">
-        <v>641</v>
+        <v>678</v>
       </c>
       <c r="C109" t="s">
-        <v>642</v>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>669</v>
+      </c>
+      <c r="B110" t="s">
+        <v>678</v>
+      </c>
+      <c r="C110" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>669</v>
+      </c>
+      <c r="B111" t="s">
+        <v>678</v>
+      </c>
+      <c r="C111" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>669</v>
+      </c>
+      <c r="B112" t="s">
+        <v>678</v>
+      </c>
+      <c r="C112" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>669</v>
+      </c>
+      <c r="B113" t="s">
+        <v>680</v>
+      </c>
+      <c r="C113" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>669</v>
+      </c>
+      <c r="B114" t="s">
+        <v>681</v>
+      </c>
+      <c r="C114" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>669</v>
+      </c>
+      <c r="B115" t="s">
+        <v>682</v>
+      </c>
+      <c r="C115" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>669</v>
+      </c>
+      <c r="B116" t="s">
+        <v>683</v>
+      </c>
+      <c r="C116" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>669</v>
+      </c>
+      <c r="B117" t="s">
+        <v>685</v>
+      </c>
+      <c r="C117" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>669</v>
+      </c>
+      <c r="B118" t="s">
+        <v>687</v>
+      </c>
+      <c r="C118" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>669</v>
+      </c>
+      <c r="B119" t="s">
+        <v>689</v>
+      </c>
+      <c r="C119" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>669</v>
+      </c>
+      <c r="B120" t="s">
+        <v>690</v>
+      </c>
+      <c r="C120" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>669</v>
+      </c>
+      <c r="B121" t="s">
+        <v>691</v>
+      </c>
+      <c r="C121" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>669</v>
+      </c>
+      <c r="B125" t="s">
+        <v>499</v>
+      </c>
+      <c r="C125" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>669</v>
+      </c>
+      <c r="B126" t="s">
+        <v>501</v>
+      </c>
+      <c r="C126" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>669</v>
+      </c>
+      <c r="B127" t="s">
+        <v>696</v>
+      </c>
+      <c r="C127" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>669</v>
+      </c>
+      <c r="B128" t="s">
+        <v>697</v>
+      </c>
+      <c r="C128" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>669</v>
+      </c>
+      <c r="B129" t="s">
+        <v>698</v>
+      </c>
+      <c r="C129" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>669</v>
+      </c>
+      <c r="B131" t="s">
+        <v>700</v>
+      </c>
+      <c r="C131" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>669</v>
+      </c>
+      <c r="B132" t="s">
+        <v>702</v>
+      </c>
+      <c r="C132" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>669</v>
+      </c>
+      <c r="B133" t="s">
+        <v>704</v>
+      </c>
+      <c r="C133" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>669</v>
+      </c>
+      <c r="B134" t="s">
+        <v>706</v>
+      </c>
+      <c r="C134" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>669</v>
+      </c>
+      <c r="B135" t="s">
+        <v>708</v>
+      </c>
+      <c r="C135" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>712</v>
+      </c>
+      <c r="C137" s="9" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>714</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update DBmapping for biogas model
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\OneDrive - UCO\Documents\GitHub\project-cali\backend\v1.0\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{677F58C1-27AF-4BD9-BDC7-55FDD274697B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31E4CF25-5B16-44CC-A931-E949F5EBFDD6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D897618-9279-432E-9423-CB4B5E4D9E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1967,18 +1967,6 @@
     <t>TE-101v</t>
   </si>
   <si>
-    <t>Moles Sustrato</t>
-  </si>
-  <si>
-    <t>Msus_exp</t>
-  </si>
-  <si>
-    <t>Concentracion Sustrato planta</t>
-  </si>
-  <si>
-    <t>Csus_exp</t>
-  </si>
-  <si>
     <t>K_mean</t>
   </si>
   <si>
@@ -2334,6 +2322,18 @@
   </si>
   <si>
     <t>M-VGT_V101</t>
+  </si>
+  <si>
+    <t>Moles Sustrato en R101</t>
+  </si>
+  <si>
+    <t>Msus_exp_R101</t>
+  </si>
+  <si>
+    <t>Csus_exp_R101</t>
+  </si>
+  <si>
+    <t>Concentracion Sustrato en R101</t>
   </si>
 </sst>
 </file>
@@ -2822,7 +2822,7 @@
         <v>440</v>
       </c>
       <c r="E5" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="F5" t="s">
         <v>527</v>
@@ -6826,7 +6826,7 @@
   <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7721,10 +7721,10 @@
         <v>528</v>
       </c>
       <c r="B81" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C81" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -7732,10 +7732,10 @@
         <v>528</v>
       </c>
       <c r="B82" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C82" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -7743,7 +7743,7 @@
         <v>528</v>
       </c>
       <c r="B83" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C83" t="s">
         <v>574</v>
@@ -7754,10 +7754,10 @@
         <v>528</v>
       </c>
       <c r="B84" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C84" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -7765,10 +7765,10 @@
         <v>528</v>
       </c>
       <c r="B85" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C85" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -7776,10 +7776,10 @@
         <v>528</v>
       </c>
       <c r="B86" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C86" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -7798,10 +7798,10 @@
         <v>528</v>
       </c>
       <c r="B88" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C88" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -7809,10 +7809,10 @@
         <v>528</v>
       </c>
       <c r="B89" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C89" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -7820,10 +7820,10 @@
         <v>528</v>
       </c>
       <c r="B90" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C90" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -7831,10 +7831,10 @@
         <v>528</v>
       </c>
       <c r="B91" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C91" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -7842,10 +7842,10 @@
         <v>528</v>
       </c>
       <c r="B92" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C92" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -7864,10 +7864,10 @@
         <v>625</v>
       </c>
       <c r="B94" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C94" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -7875,10 +7875,10 @@
         <v>625</v>
       </c>
       <c r="B95" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C95" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -7897,10 +7897,10 @@
         <v>625</v>
       </c>
       <c r="B97" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C97" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -7908,10 +7908,10 @@
         <v>625</v>
       </c>
       <c r="B98" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C98" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -7919,10 +7919,10 @@
         <v>625</v>
       </c>
       <c r="B99" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C99" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -7930,10 +7930,10 @@
         <v>625</v>
       </c>
       <c r="B100" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="C100" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -7941,10 +7941,10 @@
         <v>625</v>
       </c>
       <c r="B101" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C101" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -7952,10 +7952,10 @@
         <v>625</v>
       </c>
       <c r="B102" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C102" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -7963,10 +7963,10 @@
         <v>625</v>
       </c>
       <c r="B103" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="C103" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -7974,10 +7974,10 @@
         <v>625</v>
       </c>
       <c r="B104" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C104" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -7985,10 +7985,10 @@
         <v>625</v>
       </c>
       <c r="B105" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C105" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -7996,10 +7996,10 @@
         <v>625</v>
       </c>
       <c r="B106" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C106" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -8007,10 +8007,10 @@
         <v>625</v>
       </c>
       <c r="B107" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C107" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -8018,10 +8018,10 @@
         <v>625</v>
       </c>
       <c r="B108" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="C108" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -8029,10 +8029,10 @@
         <v>625</v>
       </c>
       <c r="B109" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C109" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -8040,10 +8040,10 @@
         <v>625</v>
       </c>
       <c r="B110" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C110" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -8051,10 +8051,10 @@
         <v>625</v>
       </c>
       <c r="B111" t="s">
-        <v>630</v>
+        <v>749</v>
       </c>
       <c r="C111" t="s">
-        <v>631</v>
+        <v>750</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -8062,10 +8062,10 @@
         <v>625</v>
       </c>
       <c r="B112" t="s">
-        <v>632</v>
+        <v>752</v>
       </c>
       <c r="C112" t="s">
-        <v>633</v>
+        <v>751</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -8073,7 +8073,7 @@
         <v>625</v>
       </c>
       <c r="B113" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C113" t="s">
         <v>552</v>
@@ -8084,7 +8084,7 @@
         <v>625</v>
       </c>
       <c r="B114" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C114" t="s">
         <v>550</v>
@@ -8095,62 +8095,62 @@
         <v>625</v>
       </c>
       <c r="B115" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C115" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="C117" s="10" t="s">
         <v>659</v>
-      </c>
-      <c r="B117" s="10" t="s">
-        <v>662</v>
-      </c>
-      <c r="C117" s="10" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B120" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C120" t="s">
         <v>473</v>
@@ -8158,10 +8158,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B121" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C121" t="s">
         <v>475</v>
@@ -8169,10 +8169,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B122" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C122" t="s">
         <v>496</v>
@@ -8180,21 +8180,21 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B123" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C123" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B124" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C124" t="s">
         <v>483</v>
@@ -8202,10 +8202,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B125" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C125" t="s">
         <v>486</v>
@@ -8213,10 +8213,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B126" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C126" t="s">
         <v>489</v>
@@ -8224,43 +8224,43 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B127" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C127" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B128" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C128" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B129" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="C129" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B130" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C130" t="s">
         <v>492</v>
@@ -8268,10 +8268,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B131" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C131" t="s">
         <v>498</v>
@@ -8279,21 +8279,21 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B132" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C132" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B133" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C133" t="s">
         <v>514</v>
@@ -8301,10 +8301,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B134" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C134" t="s">
         <v>516</v>
@@ -8312,10 +8312,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B135" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="C135" t="s">
         <v>518</v>
@@ -8323,7 +8323,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B136" t="s">
         <v>499</v>
@@ -8334,7 +8334,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B137" t="s">
         <v>501</v>
@@ -8345,10 +8345,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B138" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C138" t="s">
         <v>504</v>
@@ -8356,10 +8356,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B139" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C139" t="s">
         <v>506</v>
@@ -8367,10 +8367,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B140" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="C140" t="s">
         <v>508</v>
@@ -8378,10 +8378,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B141" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="C141" t="s">
         <v>510</v>
@@ -8389,109 +8389,109 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B142" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C142" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B143" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="C143" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B144" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C144" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B145" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C145" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B146" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C146" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B147" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C147" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B148" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C148" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B149" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="C149" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B150" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C150" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B151" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="C151" t="s">
         <v>524</v>
@@ -8499,68 +8499,68 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B152" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="C152" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B153" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C153" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B154" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C154" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B155" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C155" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B156" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="C156" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B157" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C157" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Turbine DB variables update and DC load outputs
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\OneDrive - UCO\Documents\GitHub\project-cali\backend\v1.0\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\project-cali\backend\v1.0\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D897618-9279-432E-9423-CB4B5E4D9E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9EDFB9-6152-4F53-92D9-A9C2F5936C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="764">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -1523,48 +1523,30 @@
     <t>PT002</t>
   </si>
   <si>
-    <t>Voltaje generada por turbinas (controladores de carga )</t>
-  </si>
-  <si>
     <t>VG001</t>
   </si>
   <si>
     <t>VG002</t>
   </si>
   <si>
-    <t>Corriente generada por turbinas (controladores de carga )</t>
-  </si>
-  <si>
     <t>IG001</t>
   </si>
   <si>
     <t>IG002</t>
   </si>
   <si>
-    <t>Potencia generada por las turbinas (controladores de carga )</t>
-  </si>
-  <si>
     <t>PG001</t>
   </si>
   <si>
     <t>PG002</t>
   </si>
   <si>
-    <t>Voltaje de las baterías (controladores de carga )</t>
-  </si>
-  <si>
     <t>VB001</t>
   </si>
   <si>
-    <t>Corriente de carga (controladores de carga )</t>
-  </si>
-  <si>
     <t>IC001</t>
   </si>
   <si>
-    <t>Temperatura Baterías (controladores de carga )</t>
-  </si>
-  <si>
     <t>TE003</t>
   </si>
   <si>
@@ -2334,13 +2316,64 @@
   </si>
   <si>
     <t>Concentracion Sustrato en R101</t>
+  </si>
+  <si>
+    <t>Voltaje generada por turbina Pelton (Controlador Pelton)</t>
+  </si>
+  <si>
+    <t>Voltaje generado por turbina Turgo (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>Corriente generada por turbina Pelton (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>Corriente generada por turbina Turgo (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>Potencia generada por turbina Pelton (Controlador Pelton)</t>
+  </si>
+  <si>
+    <t>Potencia generada por turbina Turgo (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>Voltaje de las baterías (Controlador Pelton)</t>
+  </si>
+  <si>
+    <t>Corriente de carga (Controlador Pelton)</t>
+  </si>
+  <si>
+    <t>Potencia de las baterías (Controlador Pelton)</t>
+  </si>
+  <si>
+    <t>Temperatura Baterías (Controlador Pelton)</t>
+  </si>
+  <si>
+    <t>Voltaje de las baterías (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>VB002</t>
+  </si>
+  <si>
+    <t>Corriente de carga (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>IC002</t>
+  </si>
+  <si>
+    <t>Potencia de las baterías  (Controlador Turgo)</t>
+  </si>
+  <si>
+    <t>PB002</t>
+  </si>
+  <si>
+    <t>Temperatura Baterías  (Controlador Turgo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2390,24 +2423,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2422,7 +2443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2434,8 +2455,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2722,13 +2742,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>275</v>
       </c>
@@ -2748,7 +2768,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>436</v>
       </c>
@@ -2768,7 +2788,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>436</v>
       </c>
@@ -2788,9 +2808,9 @@
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="B4" t="s">
         <v>437</v>
@@ -2805,10 +2825,10 @@
         <v>438</v>
       </c>
       <c r="F4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>436</v>
       </c>
@@ -2822,13 +2842,13 @@
         <v>440</v>
       </c>
       <c r="E5" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="F5" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="E10" s="8"/>
     </row>
   </sheetData>
@@ -2845,13 +2865,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>275</v>
       </c>
@@ -2865,7 +2885,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>435</v>
       </c>
@@ -2889,17 +2909,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>428</v>
       </c>
@@ -2910,7 +2930,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="1" customFormat="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2921,7 +2941,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2932,7 +2952,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2943,7 +2963,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2954,7 +2974,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2965,7 +2985,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2976,7 +2996,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2987,7 +3007,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2998,7 +3018,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3009,7 +3029,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3020,7 +3040,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3031,7 +3051,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3042,7 +3062,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3053,7 +3073,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3064,7 +3084,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3075,7 +3095,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3086,7 +3106,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3097,7 +3117,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3108,7 +3128,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3119,7 +3139,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3130,136 +3150,136 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1">
       <c r="A55" s="6"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1">
       <c r="A56" s="6"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1">
       <c r="A57" s="6"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1">
       <c r="A58" s="6"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1">
       <c r="A61" s="6"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1">
       <c r="A62" s="6"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1">
       <c r="A63" s="6"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1">
       <c r="A64" s="6"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1">
       <c r="A65" s="6"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1">
       <c r="A66" s="6"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1">
       <c r="A67" s="6"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1">
       <c r="A68" s="6"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1">
       <c r="A69" s="6"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1">
       <c r="A70" s="6"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1">
       <c r="A71" s="6"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1">
       <c r="A72" s="6"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1">
       <c r="A73" s="6"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1">
       <c r="A74" s="6"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1">
       <c r="A75" s="6"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1">
       <c r="A76" s="6"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1">
       <c r="A77" s="6"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1">
       <c r="A78" s="6"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1">
       <c r="A79" s="6"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1">
       <c r="A80" s="6"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1">
       <c r="A93" s="2"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1">
       <c r="A115" s="6"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1">
       <c r="A116" s="6"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1">
       <c r="A117" s="6"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1">
       <c r="A118" s="6"/>
     </row>
   </sheetData>
@@ -3275,18 +3295,18 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -3312,7 +3332,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3358,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3364,7 +3384,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3390,7 +3410,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3416,7 +3436,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3442,7 +3462,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3468,7 +3488,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3494,7 +3514,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3520,7 +3540,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3546,7 +3566,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3572,7 +3592,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3598,7 +3618,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3624,7 +3644,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -3650,7 +3670,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -3676,7 +3696,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -3702,7 +3722,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -3728,7 +3748,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3754,7 +3774,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -3780,7 +3800,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -3803,7 +3823,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3826,7 +3846,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -3849,7 +3869,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3875,7 +3895,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -3901,7 +3921,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3927,7 +3947,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -3953,7 +3973,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -3979,7 +3999,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -4005,7 +4025,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -4031,7 +4051,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -4057,7 +4077,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -4083,7 +4103,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -4109,7 +4129,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -4135,7 +4155,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -4161,7 +4181,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -4187,7 +4207,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -4213,7 +4233,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -4239,7 +4259,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -4265,7 +4285,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -4291,7 +4311,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -4317,7 +4337,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -4343,7 +4363,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -4369,7 +4389,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -4395,7 +4415,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -4421,7 +4441,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -4447,7 +4467,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>211</v>
       </c>
@@ -4473,7 +4493,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>212</v>
       </c>
@@ -4499,7 +4519,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>213</v>
       </c>
@@ -4525,7 +4545,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>214</v>
       </c>
@@ -4551,7 +4571,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>215</v>
       </c>
@@ -4577,7 +4597,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -4603,7 +4623,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>217</v>
       </c>
@@ -4629,7 +4649,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>218</v>
       </c>
@@ -4655,7 +4675,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>219</v>
       </c>
@@ -4681,7 +4701,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>220</v>
       </c>
@@ -4707,7 +4727,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -4733,7 +4753,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -4759,7 +4779,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -4785,7 +4805,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -4811,7 +4831,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>223</v>
       </c>
@@ -4837,7 +4857,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>224</v>
       </c>
@@ -4863,7 +4883,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -4889,7 +4909,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>226</v>
       </c>
@@ -4915,7 +4935,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>227</v>
       </c>
@@ -4941,7 +4961,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>228</v>
       </c>
@@ -4967,7 +4987,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4993,7 +5013,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>230</v>
       </c>
@@ -5019,7 +5039,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -5045,7 +5065,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -5071,7 +5091,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>233</v>
       </c>
@@ -5097,7 +5117,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -5123,7 +5143,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -5149,7 +5169,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -5175,7 +5195,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>235</v>
       </c>
@@ -5201,7 +5221,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>236</v>
       </c>
@@ -5227,7 +5247,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>237</v>
       </c>
@@ -5253,7 +5273,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>238</v>
       </c>
@@ -5279,7 +5299,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -5305,7 +5325,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>240</v>
       </c>
@@ -5331,7 +5351,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -5357,7 +5377,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>242</v>
       </c>
@@ -5383,7 +5403,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>243</v>
       </c>
@@ -5409,7 +5429,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>244</v>
       </c>
@@ -5435,7 +5455,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>245</v>
       </c>
@@ -5461,7 +5481,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>246</v>
       </c>
@@ -5487,7 +5507,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>247</v>
       </c>
@@ -5513,7 +5533,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>116</v>
       </c>
@@ -5539,7 +5559,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>118</v>
       </c>
@@ -5565,7 +5585,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>248</v>
       </c>
@@ -5591,7 +5611,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>249</v>
       </c>
@@ -5617,7 +5637,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>250</v>
       </c>
@@ -5643,7 +5663,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -5669,7 +5689,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>252</v>
       </c>
@@ -5695,7 +5715,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>253</v>
       </c>
@@ -5721,7 +5741,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>254</v>
       </c>
@@ -5747,7 +5767,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>255</v>
       </c>
@@ -5773,7 +5793,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>256</v>
       </c>
@@ -5799,7 +5819,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>257</v>
       </c>
@@ -5825,7 +5845,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>258</v>
       </c>
@@ -5851,7 +5871,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>259</v>
       </c>
@@ -5877,7 +5897,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>260</v>
       </c>
@@ -5903,7 +5923,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -5929,7 +5949,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -5955,7 +5975,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>261</v>
       </c>
@@ -5981,7 +6001,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>262</v>
       </c>
@@ -6007,7 +6027,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>263</v>
       </c>
@@ -6033,7 +6053,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>264</v>
       </c>
@@ -6059,7 +6079,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>265</v>
       </c>
@@ -6085,7 +6105,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>266</v>
       </c>
@@ -6111,7 +6131,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>267</v>
       </c>
@@ -6137,7 +6157,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>268</v>
       </c>
@@ -6163,7 +6183,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>269</v>
       </c>
@@ -6189,7 +6209,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>270</v>
       </c>
@@ -6215,7 +6235,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>271</v>
       </c>
@@ -6241,7 +6261,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>272</v>
       </c>
@@ -6267,7 +6287,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>273</v>
       </c>
@@ -6293,7 +6313,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>60</v>
       </c>
@@ -6319,7 +6339,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>62</v>
       </c>
@@ -6345,7 +6365,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>64</v>
       </c>
@@ -6371,7 +6391,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>66</v>
       </c>
@@ -6397,7 +6417,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -6423,7 +6443,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>70</v>
       </c>
@@ -6449,7 +6469,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -6475,7 +6495,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>74</v>
       </c>
@@ -6501,7 +6521,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>76</v>
       </c>
@@ -6527,7 +6547,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>78</v>
       </c>
@@ -6553,7 +6573,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>80</v>
       </c>
@@ -6579,7 +6599,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>82</v>
       </c>
@@ -6605,7 +6625,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>84</v>
       </c>
@@ -6631,7 +6651,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>86</v>
       </c>
@@ -6657,7 +6677,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8">
       <c r="A131" s="6" t="s">
         <v>88</v>
       </c>
@@ -6683,7 +6703,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8">
       <c r="A132" s="6" t="s">
         <v>90</v>
       </c>
@@ -6709,7 +6729,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8">
       <c r="A133" s="6" t="s">
         <v>92</v>
       </c>
@@ -6735,7 +6755,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8">
       <c r="A134" s="6" t="s">
         <v>94</v>
       </c>
@@ -6761,7 +6781,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>96</v>
       </c>
@@ -6787,7 +6807,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>98</v>
       </c>
@@ -6823,20 +6843,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>465</v>
       </c>
@@ -6847,7 +6867,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -6858,7 +6878,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -6869,7 +6889,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>467</v>
       </c>
@@ -6880,7 +6900,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>467</v>
       </c>
@@ -6891,7 +6911,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>467</v>
       </c>
@@ -6902,7 +6922,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>467</v>
       </c>
@@ -6913,7 +6933,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>467</v>
       </c>
@@ -6924,1643 +6944,1698 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>467</v>
       </c>
       <c r="B9" t="s">
+        <v>747</v>
+      </c>
+      <c r="C9" t="s">
         <v>482</v>
       </c>
-      <c r="C9" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>467</v>
       </c>
       <c r="B10" t="s">
-        <v>482</v>
+        <v>748</v>
       </c>
       <c r="C10" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>467</v>
       </c>
       <c r="B11" t="s">
-        <v>485</v>
+        <v>749</v>
       </c>
       <c r="C11" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>467</v>
       </c>
       <c r="B12" t="s">
+        <v>750</v>
+      </c>
+      <c r="C12" t="s">
         <v>485</v>
       </c>
-      <c r="C12" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>467</v>
       </c>
       <c r="B13" t="s">
-        <v>488</v>
+        <v>751</v>
       </c>
       <c r="C13" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>467</v>
       </c>
       <c r="B14" t="s">
-        <v>488</v>
+        <v>752</v>
       </c>
       <c r="C14" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>467</v>
       </c>
       <c r="B15" t="s">
-        <v>491</v>
+        <v>753</v>
       </c>
       <c r="C15" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>467</v>
       </c>
       <c r="B16" t="s">
-        <v>493</v>
+        <v>754</v>
       </c>
       <c r="C16" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>467</v>
       </c>
       <c r="B17" t="s">
-        <v>495</v>
+        <v>755</v>
       </c>
       <c r="C17" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>467</v>
       </c>
       <c r="B18" t="s">
-        <v>497</v>
+        <v>756</v>
       </c>
       <c r="C18" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>467</v>
       </c>
       <c r="B19" t="s">
-        <v>499</v>
+        <v>757</v>
       </c>
       <c r="C19" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>467</v>
       </c>
       <c r="B20" t="s">
-        <v>501</v>
+        <v>759</v>
       </c>
       <c r="C20" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>467</v>
       </c>
       <c r="B21" t="s">
-        <v>503</v>
+        <v>761</v>
       </c>
       <c r="C21" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>467</v>
       </c>
       <c r="B22" t="s">
-        <v>505</v>
+        <v>763</v>
       </c>
       <c r="C22" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>467</v>
       </c>
       <c r="B23" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="C23" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>493</v>
+      </c>
+      <c r="C24" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>511</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>495</v>
+      </c>
+      <c r="C25" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>497</v>
+      </c>
+      <c r="C26" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>515</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>499</v>
+      </c>
+      <c r="C27" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>517</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>501</v>
+      </c>
+      <c r="C28" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>519</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>503</v>
+      </c>
+      <c r="C29" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>505</v>
+      </c>
+      <c r="C30" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" t="s">
+        <v>507</v>
+      </c>
+      <c r="C31" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B32" t="s">
+        <v>509</v>
+      </c>
+      <c r="C32" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B33" t="s">
+        <v>511</v>
+      </c>
+      <c r="C33" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B34" t="s">
+        <v>513</v>
+      </c>
+      <c r="C34" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B35" t="s">
+        <v>515</v>
+      </c>
+      <c r="C35" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B36" t="s">
+        <v>517</v>
+      </c>
+      <c r="C36" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>522</v>
+      </c>
+      <c r="B37" t="s">
         <v>523</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C37" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>522</v>
+      </c>
+      <c r="B38" t="s">
+        <v>525</v>
+      </c>
+      <c r="C38" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>522</v>
+      </c>
+      <c r="B39" t="s">
+        <v>527</v>
+      </c>
+      <c r="C39" t="s">
         <v>528</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>522</v>
+      </c>
+      <c r="B40" t="s">
         <v>529</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C40" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>528</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>522</v>
+      </c>
+      <c r="B41" t="s">
         <v>531</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C41" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>528</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>522</v>
+      </c>
+      <c r="B42" t="s">
         <v>533</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C42" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>528</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>522</v>
+      </c>
+      <c r="B43" t="s">
         <v>535</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C43" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>528</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>522</v>
+      </c>
+      <c r="B44" t="s">
         <v>537</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C44" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>528</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>522</v>
+      </c>
+      <c r="B45" t="s">
         <v>539</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C45" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>528</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>522</v>
+      </c>
+      <c r="B46" t="s">
         <v>541</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C46" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>528</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>522</v>
+      </c>
+      <c r="B47" t="s">
         <v>543</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C47" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>528</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>522</v>
+      </c>
+      <c r="B48" t="s">
         <v>545</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C48" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>528</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>522</v>
+      </c>
+      <c r="B49" t="s">
         <v>547</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C49" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>528</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>522</v>
+      </c>
+      <c r="B50" t="s">
         <v>549</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C50" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>528</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>522</v>
+      </c>
+      <c r="B51" t="s">
         <v>551</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C51" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>528</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>522</v>
+      </c>
+      <c r="B52" t="s">
         <v>553</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C52" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>528</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>522</v>
+      </c>
+      <c r="B53" t="s">
         <v>555</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C53" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>528</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>522</v>
+      </c>
+      <c r="B54" t="s">
         <v>557</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C54" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>528</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>522</v>
+      </c>
+      <c r="B55" t="s">
         <v>559</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C55" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>528</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>522</v>
+      </c>
+      <c r="B56" t="s">
         <v>561</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C56" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>528</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>522</v>
+      </c>
+      <c r="B57" t="s">
         <v>563</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C57" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>528</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>522</v>
+      </c>
+      <c r="B58" t="s">
         <v>565</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C58" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>528</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>522</v>
+      </c>
+      <c r="B59" t="s">
         <v>567</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C59" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>528</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>522</v>
+      </c>
+      <c r="B60" t="s">
         <v>569</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C60" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>528</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>522</v>
+      </c>
+      <c r="B61" t="s">
         <v>571</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C61" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>528</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>522</v>
+      </c>
+      <c r="B62" t="s">
         <v>573</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C62" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>528</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>522</v>
+      </c>
+      <c r="B63" t="s">
         <v>575</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C63" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>528</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>522</v>
+      </c>
+      <c r="B64" t="s">
         <v>577</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C64" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>528</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>522</v>
+      </c>
+      <c r="B65" t="s">
         <v>579</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C65" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>528</v>
-      </c>
-      <c r="B58" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>522</v>
+      </c>
+      <c r="B66" t="s">
         <v>581</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C66" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>528</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>522</v>
+      </c>
+      <c r="B67" t="s">
         <v>583</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C67" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>528</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>522</v>
+      </c>
+      <c r="B68" t="s">
         <v>585</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C68" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>528</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>522</v>
+      </c>
+      <c r="B69" t="s">
         <v>587</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C69" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>528</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>522</v>
+      </c>
+      <c r="B70" t="s">
         <v>589</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C70" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>528</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>522</v>
+      </c>
+      <c r="B71" t="s">
         <v>591</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C71" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>528</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>522</v>
+      </c>
+      <c r="B72" t="s">
         <v>593</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C72" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>528</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>522</v>
+      </c>
+      <c r="B73" t="s">
         <v>595</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C73" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>528</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>522</v>
+      </c>
+      <c r="B74" t="s">
         <v>597</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C74" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>528</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>522</v>
+      </c>
+      <c r="B75" t="s">
         <v>599</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C75" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>528</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>522</v>
+      </c>
+      <c r="B76" t="s">
         <v>601</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C76" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>528</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>522</v>
+      </c>
+      <c r="B77" t="s">
         <v>603</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C77" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>528</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>522</v>
+      </c>
+      <c r="B78" t="s">
         <v>605</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C78" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>528</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>522</v>
+      </c>
+      <c r="B79" t="s">
         <v>607</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C79" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>528</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>522</v>
+      </c>
+      <c r="B80" t="s">
         <v>609</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C80" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>528</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>522</v>
+      </c>
+      <c r="B81" t="s">
         <v>611</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C81" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>528</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>522</v>
+      </c>
+      <c r="B82" t="s">
         <v>613</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C82" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>528</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>522</v>
+      </c>
+      <c r="B83" t="s">
         <v>615</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C83" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>528</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>522</v>
+      </c>
+      <c r="B84" t="s">
+        <v>523</v>
+      </c>
+      <c r="C84" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>522</v>
+      </c>
+      <c r="B85" t="s">
         <v>617</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C85" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>528</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>522</v>
+      </c>
+      <c r="B86" t="s">
+        <v>627</v>
+      </c>
+      <c r="C86" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>522</v>
+      </c>
+      <c r="B87" t="s">
+        <v>629</v>
+      </c>
+      <c r="C87" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>522</v>
+      </c>
+      <c r="B88" t="s">
+        <v>631</v>
+      </c>
+      <c r="C88" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>522</v>
+      </c>
+      <c r="B89" t="s">
+        <v>632</v>
+      </c>
+      <c r="C89" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>522</v>
+      </c>
+      <c r="B90" t="s">
+        <v>634</v>
+      </c>
+      <c r="C90" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>522</v>
+      </c>
+      <c r="B91" t="s">
+        <v>636</v>
+      </c>
+      <c r="C91" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>522</v>
+      </c>
+      <c r="B92" t="s">
+        <v>593</v>
+      </c>
+      <c r="C92" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>522</v>
+      </c>
+      <c r="B93" t="s">
+        <v>637</v>
+      </c>
+      <c r="C93" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>522</v>
+      </c>
+      <c r="B94" t="s">
+        <v>639</v>
+      </c>
+      <c r="C94" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>522</v>
+      </c>
+      <c r="B95" t="s">
+        <v>641</v>
+      </c>
+      <c r="C95" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>522</v>
+      </c>
+      <c r="B96" t="s">
+        <v>643</v>
+      </c>
+      <c r="C96" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>522</v>
+      </c>
+      <c r="B97" t="s">
+        <v>645</v>
+      </c>
+      <c r="C97" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
         <v>619</v>
       </c>
-      <c r="C77" t="s">
+      <c r="B98" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>528</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="C98" t="s">
         <v>621</v>
       </c>
-      <c r="C78" t="s">
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>619</v>
+      </c>
+      <c r="B99" t="s">
+        <v>711</v>
+      </c>
+      <c r="C99" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>619</v>
+      </c>
+      <c r="B100" t="s">
+        <v>713</v>
+      </c>
+      <c r="C100" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>619</v>
+      </c>
+      <c r="B101" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>528</v>
-      </c>
-      <c r="B79" t="s">
-        <v>529</v>
-      </c>
-      <c r="C79" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>528</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="C101" t="s">
         <v>623</v>
       </c>
-      <c r="C80" t="s">
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>619</v>
+      </c>
+      <c r="B102" t="s">
+        <v>715</v>
+      </c>
+      <c r="C102" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>619</v>
+      </c>
+      <c r="B103" t="s">
+        <v>728</v>
+      </c>
+      <c r="C103" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>619</v>
+      </c>
+      <c r="B104" t="s">
+        <v>729</v>
+      </c>
+      <c r="C104" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>619</v>
+      </c>
+      <c r="B105" t="s">
+        <v>730</v>
+      </c>
+      <c r="C105" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>619</v>
+      </c>
+      <c r="B106" t="s">
+        <v>731</v>
+      </c>
+      <c r="C106" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>619</v>
+      </c>
+      <c r="B107" t="s">
+        <v>732</v>
+      </c>
+      <c r="C107" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>619</v>
+      </c>
+      <c r="B108" t="s">
+        <v>733</v>
+      </c>
+      <c r="C108" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>619</v>
+      </c>
+      <c r="B109" t="s">
+        <v>734</v>
+      </c>
+      <c r="C109" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>619</v>
+      </c>
+      <c r="B110" t="s">
+        <v>735</v>
+      </c>
+      <c r="C110" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>619</v>
+      </c>
+      <c r="B111" t="s">
+        <v>736</v>
+      </c>
+      <c r="C111" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>619</v>
+      </c>
+      <c r="B112" t="s">
+        <v>737</v>
+      </c>
+      <c r="C112" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>619</v>
+      </c>
+      <c r="B113" t="s">
+        <v>738</v>
+      </c>
+      <c r="C113" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>619</v>
+      </c>
+      <c r="B114" t="s">
+        <v>739</v>
+      </c>
+      <c r="C114" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>619</v>
+      </c>
+      <c r="B115" t="s">
+        <v>740</v>
+      </c>
+      <c r="C115" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>619</v>
+      </c>
+      <c r="B116" t="s">
+        <v>743</v>
+      </c>
+      <c r="C116" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="B120" s="9" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>528</v>
-      </c>
-      <c r="B81" t="s">
-        <v>633</v>
-      </c>
-      <c r="C81" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>528</v>
-      </c>
-      <c r="B82" t="s">
-        <v>635</v>
-      </c>
-      <c r="C82" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>528</v>
-      </c>
-      <c r="B83" t="s">
-        <v>637</v>
-      </c>
-      <c r="C83" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>528</v>
-      </c>
-      <c r="B84" t="s">
-        <v>638</v>
-      </c>
-      <c r="C84" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>528</v>
-      </c>
-      <c r="B85" t="s">
-        <v>640</v>
-      </c>
-      <c r="C85" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>528</v>
-      </c>
-      <c r="B86" t="s">
-        <v>642</v>
-      </c>
-      <c r="C86" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>528</v>
-      </c>
-      <c r="B87" t="s">
-        <v>599</v>
-      </c>
-      <c r="C87" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>528</v>
-      </c>
-      <c r="B88" t="s">
-        <v>643</v>
-      </c>
-      <c r="C88" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>528</v>
-      </c>
-      <c r="B89" t="s">
-        <v>645</v>
-      </c>
-      <c r="C89" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>528</v>
-      </c>
-      <c r="B90" t="s">
-        <v>647</v>
-      </c>
-      <c r="C90" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>528</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C120" s="9" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="9" t="s">
         <v>649</v>
       </c>
-      <c r="C91" t="s">
+      <c r="B121" s="9" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>528</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C121" s="9" t="s">
         <v>651</v>
       </c>
-      <c r="C92" t="s">
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B122" s="9" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>625</v>
-      </c>
-      <c r="B93" t="s">
-        <v>626</v>
-      </c>
-      <c r="C93" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>625</v>
-      </c>
-      <c r="B94" t="s">
-        <v>717</v>
-      </c>
-      <c r="C94" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>625</v>
-      </c>
-      <c r="B95" t="s">
-        <v>719</v>
-      </c>
-      <c r="C95" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>625</v>
-      </c>
-      <c r="B96" t="s">
-        <v>628</v>
-      </c>
-      <c r="C96" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>625</v>
-      </c>
-      <c r="B97" t="s">
-        <v>721</v>
-      </c>
-      <c r="C97" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>625</v>
-      </c>
-      <c r="B98" t="s">
-        <v>734</v>
-      </c>
-      <c r="C98" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>625</v>
-      </c>
-      <c r="B99" t="s">
-        <v>735</v>
-      </c>
-      <c r="C99" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>625</v>
-      </c>
-      <c r="B100" t="s">
-        <v>736</v>
-      </c>
-      <c r="C100" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>625</v>
-      </c>
-      <c r="B101" t="s">
-        <v>737</v>
-      </c>
-      <c r="C101" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>625</v>
-      </c>
-      <c r="B102" t="s">
-        <v>738</v>
-      </c>
-      <c r="C102" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>625</v>
-      </c>
-      <c r="B103" t="s">
-        <v>739</v>
-      </c>
-      <c r="C103" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>625</v>
-      </c>
-      <c r="B104" t="s">
-        <v>740</v>
-      </c>
-      <c r="C104" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>625</v>
-      </c>
-      <c r="B105" t="s">
-        <v>741</v>
-      </c>
-      <c r="C105" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>625</v>
-      </c>
-      <c r="B106" t="s">
-        <v>742</v>
-      </c>
-      <c r="C106" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>625</v>
-      </c>
-      <c r="B107" t="s">
-        <v>743</v>
-      </c>
-      <c r="C107" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>625</v>
-      </c>
-      <c r="B108" t="s">
-        <v>744</v>
-      </c>
-      <c r="C108" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>625</v>
-      </c>
-      <c r="B109" t="s">
-        <v>745</v>
-      </c>
-      <c r="C109" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>625</v>
-      </c>
-      <c r="B110" t="s">
-        <v>746</v>
-      </c>
-      <c r="C110" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>625</v>
-      </c>
-      <c r="B111" t="s">
-        <v>749</v>
-      </c>
-      <c r="C111" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>625</v>
-      </c>
-      <c r="B112" t="s">
-        <v>752</v>
-      </c>
-      <c r="C112" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>625</v>
-      </c>
-      <c r="B113" t="s">
+      <c r="C122" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="C113" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>625</v>
-      </c>
-      <c r="B114" t="s">
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B123" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="C114" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>625</v>
-      </c>
-      <c r="B115" t="s">
-        <v>630</v>
-      </c>
-      <c r="C115" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="10" t="s">
+      <c r="C123" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="B116" s="10" t="s">
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="B124" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="C116" s="10" t="s">
+      <c r="C124" s="9" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="B117" s="10" t="s">
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>649</v>
+      </c>
+      <c r="B125" t="s">
         <v>658</v>
       </c>
-      <c r="C117" s="10" t="s">
+      <c r="C125" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>649</v>
+      </c>
+      <c r="B126" t="s">
+        <v>658</v>
+      </c>
+      <c r="C126" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>649</v>
+      </c>
+      <c r="B127" t="s">
+        <v>658</v>
+      </c>
+      <c r="C127" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>649</v>
+      </c>
+      <c r="B128" t="s">
+        <v>658</v>
+      </c>
+      <c r="C128" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="B118" s="10" t="s">
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>649</v>
+      </c>
+      <c r="B129" t="s">
         <v>660</v>
       </c>
-      <c r="C118" s="10" t="s">
+      <c r="C129" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>649</v>
+      </c>
+      <c r="B130" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="B119" s="10" t="s">
+      <c r="C130" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>649</v>
+      </c>
+      <c r="B131" t="s">
         <v>662</v>
       </c>
-      <c r="C119" s="10" t="s">
+      <c r="C131" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>649</v>
+      </c>
+      <c r="B132" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>655</v>
-      </c>
-      <c r="B120" t="s">
+      <c r="C132" t="s">
         <v>664</v>
       </c>
-      <c r="C120" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>655</v>
-      </c>
-      <c r="B121" t="s">
-        <v>664</v>
-      </c>
-      <c r="C121" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>655</v>
-      </c>
-      <c r="B122" t="s">
-        <v>664</v>
-      </c>
-      <c r="C122" t="s">
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>649</v>
+      </c>
+      <c r="B133" t="s">
+        <v>665</v>
+      </c>
+      <c r="C133" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>649</v>
+      </c>
+      <c r="B134" t="s">
+        <v>667</v>
+      </c>
+      <c r="C134" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>649</v>
+      </c>
+      <c r="B135" t="s">
+        <v>669</v>
+      </c>
+      <c r="C135" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>649</v>
+      </c>
+      <c r="B136" t="s">
+        <v>670</v>
+      </c>
+      <c r="C136" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>649</v>
+      </c>
+      <c r="B137" t="s">
+        <v>671</v>
+      </c>
+      <c r="C137" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>649</v>
+      </c>
+      <c r="B138" t="s">
+        <v>673</v>
+      </c>
+      <c r="C138" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>649</v>
+      </c>
+      <c r="B139" t="s">
+        <v>674</v>
+      </c>
+      <c r="C139" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>649</v>
+      </c>
+      <c r="B140" t="s">
+        <v>675</v>
+      </c>
+      <c r="C140" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>649</v>
+      </c>
+      <c r="B141" t="s">
+        <v>493</v>
+      </c>
+      <c r="C141" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>649</v>
+      </c>
+      <c r="B142" t="s">
+        <v>495</v>
+      </c>
+      <c r="C142" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>655</v>
-      </c>
-      <c r="B123" t="s">
-        <v>664</v>
-      </c>
-      <c r="C123" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>655</v>
-      </c>
-      <c r="B124" t="s">
-        <v>666</v>
-      </c>
-      <c r="C124" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>655</v>
-      </c>
-      <c r="B125" t="s">
-        <v>667</v>
-      </c>
-      <c r="C125" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>655</v>
-      </c>
-      <c r="B126" t="s">
-        <v>668</v>
-      </c>
-      <c r="C126" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>655</v>
-      </c>
-      <c r="B127" t="s">
-        <v>669</v>
-      </c>
-      <c r="C127" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>655</v>
-      </c>
-      <c r="B128" t="s">
-        <v>671</v>
-      </c>
-      <c r="C128" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>655</v>
-      </c>
-      <c r="B129" t="s">
-        <v>673</v>
-      </c>
-      <c r="C129" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>655</v>
-      </c>
-      <c r="B130" t="s">
-        <v>675</v>
-      </c>
-      <c r="C130" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>655</v>
-      </c>
-      <c r="B131" t="s">
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>649</v>
+      </c>
+      <c r="B143" t="s">
         <v>676</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C143" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>655</v>
-      </c>
-      <c r="B132" t="s">
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>649</v>
+      </c>
+      <c r="B144" t="s">
         <v>677</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C144" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>649</v>
+      </c>
+      <c r="B145" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>655</v>
-      </c>
-      <c r="B133" t="s">
+      <c r="C145" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>649</v>
+      </c>
+      <c r="B146" t="s">
         <v>679</v>
       </c>
-      <c r="C133" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>655</v>
-      </c>
-      <c r="B134" t="s">
+      <c r="C146" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>649</v>
+      </c>
+      <c r="B147" t="s">
         <v>680</v>
       </c>
-      <c r="C134" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>655</v>
-      </c>
-      <c r="B135" t="s">
+      <c r="C147" t="s">
         <v>681</v>
       </c>
-      <c r="C135" t="s">
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>649</v>
+      </c>
+      <c r="B148" t="s">
+        <v>682</v>
+      </c>
+      <c r="C148" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>649</v>
+      </c>
+      <c r="B149" t="s">
+        <v>684</v>
+      </c>
+      <c r="C149" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>649</v>
+      </c>
+      <c r="B150" t="s">
+        <v>686</v>
+      </c>
+      <c r="C150" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>649</v>
+      </c>
+      <c r="B151" t="s">
+        <v>688</v>
+      </c>
+      <c r="C151" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>649</v>
+      </c>
+      <c r="B152" t="s">
+        <v>690</v>
+      </c>
+      <c r="C152" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>649</v>
+      </c>
+      <c r="B153" t="s">
+        <v>692</v>
+      </c>
+      <c r="C153" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>649</v>
+      </c>
+      <c r="B154" t="s">
+        <v>694</v>
+      </c>
+      <c r="C154" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>649</v>
+      </c>
+      <c r="B155" t="s">
+        <v>696</v>
+      </c>
+      <c r="C155" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>649</v>
+      </c>
+      <c r="B156" t="s">
+        <v>698</v>
+      </c>
+      <c r="C156" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>655</v>
-      </c>
-      <c r="B136" t="s">
-        <v>499</v>
-      </c>
-      <c r="C136" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>655</v>
-      </c>
-      <c r="B137" t="s">
-        <v>501</v>
-      </c>
-      <c r="C137" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>655</v>
-      </c>
-      <c r="B138" t="s">
-        <v>682</v>
-      </c>
-      <c r="C138" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>655</v>
-      </c>
-      <c r="B139" t="s">
-        <v>683</v>
-      </c>
-      <c r="C139" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>655</v>
-      </c>
-      <c r="B140" t="s">
-        <v>684</v>
-      </c>
-      <c r="C140" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>655</v>
-      </c>
-      <c r="B141" t="s">
-        <v>685</v>
-      </c>
-      <c r="C141" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>655</v>
-      </c>
-      <c r="B142" t="s">
-        <v>686</v>
-      </c>
-      <c r="C142" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>655</v>
-      </c>
-      <c r="B143" t="s">
-        <v>688</v>
-      </c>
-      <c r="C143" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>655</v>
-      </c>
-      <c r="B144" t="s">
-        <v>690</v>
-      </c>
-      <c r="C144" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>655</v>
-      </c>
-      <c r="B145" t="s">
-        <v>692</v>
-      </c>
-      <c r="C145" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>655</v>
-      </c>
-      <c r="B146" t="s">
-        <v>694</v>
-      </c>
-      <c r="C146" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>655</v>
-      </c>
-      <c r="B147" t="s">
-        <v>696</v>
-      </c>
-      <c r="C147" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>655</v>
-      </c>
-      <c r="B148" t="s">
-        <v>698</v>
-      </c>
-      <c r="C148" t="s">
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>649</v>
+      </c>
+      <c r="B157" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>655</v>
-      </c>
-      <c r="B149" t="s">
+      <c r="C157" t="s">
         <v>700</v>
       </c>
-      <c r="C149" t="s">
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>649</v>
+      </c>
+      <c r="B158" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>655</v>
-      </c>
-      <c r="B150" t="s">
+      <c r="C158" t="s">
         <v>702</v>
       </c>
-      <c r="C150" t="s">
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>649</v>
+      </c>
+      <c r="B159" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>655</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="C159" t="s">
         <v>704</v>
       </c>
-      <c r="C151" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>655</v>
-      </c>
-      <c r="B152" t="s">
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>649</v>
+      </c>
+      <c r="B160" t="s">
         <v>705</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C160" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>655</v>
-      </c>
-      <c r="B153" t="s">
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>649</v>
+      </c>
+      <c r="B161" t="s">
+        <v>710</v>
+      </c>
+      <c r="C161" t="s">
         <v>707</v>
       </c>
-      <c r="C153" t="s">
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>649</v>
+      </c>
+      <c r="B162" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>655</v>
-      </c>
-      <c r="B154" t="s">
+      <c r="C162" t="s">
         <v>709</v>
-      </c>
-      <c r="C154" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>655</v>
-      </c>
-      <c r="B155" t="s">
-        <v>711</v>
-      </c>
-      <c r="C155" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>655</v>
-      </c>
-      <c r="B156" t="s">
-        <v>716</v>
-      </c>
-      <c r="C156" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>655</v>
-      </c>
-      <c r="B157" t="s">
-        <v>714</v>
-      </c>
-      <c r="C157" t="s">
-        <v>715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Biogas Model _ Operation mode 2
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{331D2257-B55E-4DAE-AFAE-DAF991BCA6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4F4FDE4-51EB-4C16-BE57-0BE5213133B8}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{A422AA3E-2406-46D5-AC4C-5B2877F8707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C341B10-F92C-4F76-9797-E6F4E41E8671}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="829">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -2373,6 +2373,195 @@
   </si>
   <si>
     <t>TT-104</t>
+  </si>
+  <si>
+    <t>M-SV_R101</t>
+  </si>
+  <si>
+    <t>M-ST_R101</t>
+  </si>
+  <si>
+    <t>Volumen normal de biogás en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M_VGA_V102</t>
+  </si>
+  <si>
+    <t>Volumen parcial  metano en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_CH4_V102</t>
+  </si>
+  <si>
+    <t>Volumen parcial de dióxido de carbono en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_CO2_V102</t>
+  </si>
+  <si>
+    <t>Volumen parcial  sulfuro de hidrogeno en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_H2S_V102</t>
+  </si>
+  <si>
+    <t>M-PA_O2_V102</t>
+  </si>
+  <si>
+    <t>Volumen parcial  oxigeno en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_H2_V102</t>
+  </si>
+  <si>
+    <t>moles metano en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_CH4_V102</t>
+  </si>
+  <si>
+    <t>moles dioxido de carbono en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_CO2_V102</t>
+  </si>
+  <si>
+    <t>moles sulfuro de hidrógeno en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_H2S_V102</t>
+  </si>
+  <si>
+    <t>moles oxigeno en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_O2_V102</t>
+  </si>
+  <si>
+    <t>moles hidrogeno en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_H2_V102</t>
+  </si>
+  <si>
+    <t>moles agua en V102 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_H2O_V102</t>
+  </si>
+  <si>
+    <t>Presión acumulada en V102</t>
+  </si>
+  <si>
+    <t>P_acum_V102</t>
+  </si>
+  <si>
+    <t>Volumen normal acumulado en V102 (Total)</t>
+  </si>
+  <si>
+    <t>M-VGT_V102</t>
+  </si>
+  <si>
+    <t>Volumen normal de biogás en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M_VGA_V107</t>
+  </si>
+  <si>
+    <t>Volumen parcial  metano en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_CH4_V107</t>
+  </si>
+  <si>
+    <t>Volumen parcial de dióxido de carbono en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_CO2_V107</t>
+  </si>
+  <si>
+    <t>Volumen parcial  sulfuro de hidrogeno en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_H2S_V107</t>
+  </si>
+  <si>
+    <t>Volumen parcial  oxigeno en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_O2_V107</t>
+  </si>
+  <si>
+    <t>Volumen parcial hiodrogeno en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-PA_H2_V107</t>
+  </si>
+  <si>
+    <t>moles metano en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_CH4_V107</t>
+  </si>
+  <si>
+    <t>moles dioxido de carbono en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_CO2_V107</t>
+  </si>
+  <si>
+    <t>moles sulfuro de hidrógeno en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_H2S_V107</t>
+  </si>
+  <si>
+    <t>moles agua en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>moles hidrogeno en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_H2_V107</t>
+  </si>
+  <si>
+    <t>M-molA_O2_V107</t>
+  </si>
+  <si>
+    <t>moles oxigeno en V107 (almacenadas)</t>
+  </si>
+  <si>
+    <t>M-molA_H2O_V107</t>
+  </si>
+  <si>
+    <t>Presión acumulada en V107</t>
+  </si>
+  <si>
+    <t>P_acum_V107</t>
+  </si>
+  <si>
+    <t>Volumen normal acumulado en V107 (Total)</t>
+  </si>
+  <si>
+    <t>M-VGT_V107</t>
+  </si>
+  <si>
+    <t>moles metano acumulado en V101 (total)</t>
+  </si>
+  <si>
+    <t>M-molT_CH4_V101</t>
+  </si>
+  <si>
+    <t>M-molT_CH4_V102</t>
+  </si>
+  <si>
+    <t>moles metano acumulado en V102 (total)</t>
+  </si>
+  <si>
+    <t>moles metano acumulado en V107 (total)</t>
+  </si>
+  <si>
+    <t>M-molT_CH4_V107</t>
   </si>
 </sst>
 </file>
@@ -2449,7 +2638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2461,6 +2650,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6848,10 +7038,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8142,10 +8332,10 @@
         <v>619</v>
       </c>
       <c r="B117" t="s">
-        <v>741</v>
+        <v>823</v>
       </c>
       <c r="C117" t="s">
-        <v>742</v>
+        <v>824</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -8153,10 +8343,10 @@
         <v>619</v>
       </c>
       <c r="B118" t="s">
-        <v>744</v>
+        <v>768</v>
       </c>
       <c r="C118" t="s">
-        <v>743</v>
+        <v>769</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -8164,10 +8354,10 @@
         <v>619</v>
       </c>
       <c r="B119" t="s">
-        <v>762</v>
+        <v>770</v>
       </c>
       <c r="C119" t="s">
-        <v>546</v>
+        <v>771</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -8175,10 +8365,10 @@
         <v>619</v>
       </c>
       <c r="B120" t="s">
-        <v>763</v>
+        <v>772</v>
       </c>
       <c r="C120" t="s">
-        <v>544</v>
+        <v>773</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -8186,439 +8376,445 @@
         <v>619</v>
       </c>
       <c r="B121" t="s">
-        <v>624</v>
+        <v>774</v>
       </c>
       <c r="C121" t="s">
-        <v>625</v>
+        <v>775</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B122" t="s">
-        <v>648</v>
+        <v>777</v>
       </c>
       <c r="C122" t="s">
-        <v>649</v>
+        <v>776</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B123" t="s">
-        <v>650</v>
+        <v>730</v>
       </c>
       <c r="C123" t="s">
-        <v>651</v>
+        <v>778</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B124" t="s">
-        <v>652</v>
+        <v>779</v>
       </c>
       <c r="C124" t="s">
-        <v>653</v>
+        <v>780</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B125" t="s">
-        <v>654</v>
+        <v>781</v>
       </c>
       <c r="C125" t="s">
-        <v>655</v>
+        <v>782</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B126" t="s">
-        <v>656</v>
+        <v>783</v>
       </c>
       <c r="C126" t="s">
-        <v>473</v>
+        <v>784</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B127" t="s">
-        <v>656</v>
+        <v>785</v>
       </c>
       <c r="C127" t="s">
-        <v>475</v>
+        <v>786</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B128" t="s">
-        <v>656</v>
+        <v>787</v>
       </c>
       <c r="C128" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B129" t="s">
-        <v>656</v>
+        <v>789</v>
       </c>
       <c r="C129" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B130" t="s">
-        <v>658</v>
+        <v>791</v>
       </c>
       <c r="C130" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B131" t="s">
-        <v>659</v>
+        <v>793</v>
       </c>
       <c r="C131" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B132" t="s">
-        <v>660</v>
+        <v>826</v>
       </c>
       <c r="C132" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B133" t="s">
-        <v>661</v>
+        <v>795</v>
       </c>
       <c r="C133" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B134" t="s">
-        <v>663</v>
+        <v>797</v>
       </c>
       <c r="C134" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B135" t="s">
-        <v>665</v>
+        <v>799</v>
       </c>
       <c r="C135" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B136" t="s">
-        <v>667</v>
+        <v>801</v>
       </c>
       <c r="C136" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B137" t="s">
-        <v>668</v>
+        <v>803</v>
       </c>
       <c r="C137" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B138" t="s">
-        <v>669</v>
+        <v>805</v>
       </c>
       <c r="C138" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B139" t="s">
-        <v>671</v>
+        <v>807</v>
       </c>
       <c r="C139" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B140" t="s">
-        <v>672</v>
+        <v>809</v>
       </c>
       <c r="C140" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B141" t="s">
-        <v>673</v>
+        <v>811</v>
       </c>
       <c r="C141" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B142" t="s">
-        <v>493</v>
+        <v>817</v>
       </c>
       <c r="C142" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B143" t="s">
-        <v>495</v>
+        <v>814</v>
       </c>
       <c r="C143" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+        <v>815</v>
+      </c>
+      <c r="E143" s="9"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B144" t="s">
-        <v>674</v>
+        <v>813</v>
       </c>
       <c r="C144" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B145" t="s">
-        <v>675</v>
+        <v>819</v>
       </c>
       <c r="C145" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+        <v>820</v>
+      </c>
+      <c r="D145" s="9"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B146" t="s">
-        <v>676</v>
+        <v>821</v>
       </c>
       <c r="C146" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B147" t="s">
-        <v>677</v>
+        <v>827</v>
       </c>
       <c r="C147" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+        <v>828</v>
+      </c>
+      <c r="F147" s="8"/>
+      <c r="G147" s="9"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B148" t="s">
-        <v>678</v>
+        <v>741</v>
       </c>
       <c r="C148" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+        <v>742</v>
+      </c>
+      <c r="F148" s="8"/>
+      <c r="G148" s="9"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B149" t="s">
-        <v>680</v>
+        <v>744</v>
       </c>
       <c r="C149" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B150" t="s">
-        <v>682</v>
+        <v>762</v>
       </c>
       <c r="C150" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B151" t="s">
-        <v>684</v>
+        <v>763</v>
       </c>
       <c r="C151" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B152" t="s">
-        <v>686</v>
+        <v>624</v>
       </c>
       <c r="C152" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>647</v>
       </c>
       <c r="B153" t="s">
-        <v>688</v>
+        <v>648</v>
       </c>
       <c r="C153" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>647</v>
       </c>
       <c r="B154" t="s">
-        <v>690</v>
+        <v>650</v>
       </c>
       <c r="C154" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>647</v>
       </c>
       <c r="B155" t="s">
-        <v>692</v>
+        <v>652</v>
       </c>
       <c r="C155" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>647</v>
       </c>
       <c r="B156" t="s">
-        <v>694</v>
+        <v>654</v>
       </c>
       <c r="C156" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>647</v>
       </c>
       <c r="B157" t="s">
-        <v>696</v>
+        <v>656</v>
       </c>
       <c r="C157" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>647</v>
       </c>
       <c r="B158" t="s">
-        <v>697</v>
+        <v>656</v>
       </c>
       <c r="C158" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>647</v>
       </c>
       <c r="B159" t="s">
-        <v>699</v>
+        <v>656</v>
       </c>
       <c r="C159" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>647</v>
       </c>
       <c r="B160" t="s">
-        <v>701</v>
+        <v>656</v>
       </c>
       <c r="C160" t="s">
-        <v>702</v>
+        <v>657</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -8626,10 +8822,10 @@
         <v>647</v>
       </c>
       <c r="B161" t="s">
-        <v>703</v>
+        <v>658</v>
       </c>
       <c r="C161" t="s">
-        <v>704</v>
+        <v>482</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -8637,10 +8833,10 @@
         <v>647</v>
       </c>
       <c r="B162" t="s">
-        <v>708</v>
+        <v>659</v>
       </c>
       <c r="C162" t="s">
-        <v>705</v>
+        <v>484</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -8648,9 +8844,350 @@
         <v>647</v>
       </c>
       <c r="B163" t="s">
+        <v>660</v>
+      </c>
+      <c r="C163" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>647</v>
+      </c>
+      <c r="B164" t="s">
+        <v>661</v>
+      </c>
+      <c r="C164" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>647</v>
+      </c>
+      <c r="B165" t="s">
+        <v>663</v>
+      </c>
+      <c r="C165" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>647</v>
+      </c>
+      <c r="B166" t="s">
+        <v>665</v>
+      </c>
+      <c r="C166" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>647</v>
+      </c>
+      <c r="B167" t="s">
+        <v>667</v>
+      </c>
+      <c r="C167" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>647</v>
+      </c>
+      <c r="B168" t="s">
+        <v>668</v>
+      </c>
+      <c r="C168" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>647</v>
+      </c>
+      <c r="B169" t="s">
+        <v>669</v>
+      </c>
+      <c r="C169" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>647</v>
+      </c>
+      <c r="B170" t="s">
+        <v>671</v>
+      </c>
+      <c r="C170" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>647</v>
+      </c>
+      <c r="B171" t="s">
+        <v>672</v>
+      </c>
+      <c r="C171" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>647</v>
+      </c>
+      <c r="B172" t="s">
+        <v>673</v>
+      </c>
+      <c r="C172" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>647</v>
+      </c>
+      <c r="B173" t="s">
+        <v>493</v>
+      </c>
+      <c r="C173" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>647</v>
+      </c>
+      <c r="B174" t="s">
+        <v>495</v>
+      </c>
+      <c r="C174" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>647</v>
+      </c>
+      <c r="B175" t="s">
+        <v>674</v>
+      </c>
+      <c r="C175" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>647</v>
+      </c>
+      <c r="B176" t="s">
+        <v>675</v>
+      </c>
+      <c r="C176" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>647</v>
+      </c>
+      <c r="B177" t="s">
+        <v>676</v>
+      </c>
+      <c r="C177" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>647</v>
+      </c>
+      <c r="B178" t="s">
+        <v>677</v>
+      </c>
+      <c r="C178" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>647</v>
+      </c>
+      <c r="B179" t="s">
+        <v>678</v>
+      </c>
+      <c r="C179" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>647</v>
+      </c>
+      <c r="B180" t="s">
+        <v>680</v>
+      </c>
+      <c r="C180" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>647</v>
+      </c>
+      <c r="B181" t="s">
+        <v>682</v>
+      </c>
+      <c r="C181" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>647</v>
+      </c>
+      <c r="B182" t="s">
+        <v>684</v>
+      </c>
+      <c r="C182" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>647</v>
+      </c>
+      <c r="B183" t="s">
+        <v>686</v>
+      </c>
+      <c r="C183" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>647</v>
+      </c>
+      <c r="B184" t="s">
+        <v>688</v>
+      </c>
+      <c r="C184" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>647</v>
+      </c>
+      <c r="B185" t="s">
+        <v>690</v>
+      </c>
+      <c r="C185" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>647</v>
+      </c>
+      <c r="B186" t="s">
+        <v>692</v>
+      </c>
+      <c r="C186" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>647</v>
+      </c>
+      <c r="B187" t="s">
+        <v>694</v>
+      </c>
+      <c r="C187" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>647</v>
+      </c>
+      <c r="B188" t="s">
+        <v>696</v>
+      </c>
+      <c r="C188" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>647</v>
+      </c>
+      <c r="B189" t="s">
+        <v>697</v>
+      </c>
+      <c r="C189" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>647</v>
+      </c>
+      <c r="B190" t="s">
+        <v>699</v>
+      </c>
+      <c r="C190" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>647</v>
+      </c>
+      <c r="B191" t="s">
+        <v>701</v>
+      </c>
+      <c r="C191" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>647</v>
+      </c>
+      <c r="B192" t="s">
+        <v>703</v>
+      </c>
+      <c r="C192" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>647</v>
+      </c>
+      <c r="B193" t="s">
+        <v>708</v>
+      </c>
+      <c r="C193" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>647</v>
+      </c>
+      <c r="B194" t="s">
         <v>706</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C194" t="s">
         <v>707</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Operation Mode 4 in biogas (pumps configuration and reactors configuration)
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{A422AA3E-2406-46D5-AC4C-5B2877F8707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{066571DD-7F70-40F4-B8B9-E22E449EF5B3}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{A422AA3E-2406-46D5-AC4C-5B2877F8707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68D54FD1-92A6-410D-8342-1B2B73129CB9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="836">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -2363,9 +2363,6 @@
     <t>Temperatura Baterías  (Controlador Turgo)</t>
   </si>
   <si>
-    <t>concentración de dolidos volátiles a la salida de R101</t>
-  </si>
-  <si>
     <t>concentracion de sólidos totales a la salida de R101</t>
   </si>
   <si>
@@ -2571,6 +2568,21 @@
   </si>
   <si>
     <t>Msus_exp_R102</t>
+  </si>
+  <si>
+    <t>concentración de solidos volátiles a la salida de R101</t>
+  </si>
+  <si>
+    <t>concentración de solidos volátiles a la salida de R102</t>
+  </si>
+  <si>
+    <t>M-SV_R102</t>
+  </si>
+  <si>
+    <t>concentracion de sólidos totales a la salida de R102</t>
+  </si>
+  <si>
+    <t>M-ST_R102</t>
   </si>
 </sst>
 </file>
@@ -7050,10 +7062,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:G196"/>
+  <dimension ref="A1:G198"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G148" sqref="G148"/>
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7838,10 +7850,10 @@
         <v>522</v>
       </c>
       <c r="B71" t="s">
+        <v>763</v>
+      </c>
+      <c r="C71" t="s">
         <v>764</v>
-      </c>
-      <c r="C71" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -8344,10 +8356,10 @@
         <v>619</v>
       </c>
       <c r="B117" t="s">
+        <v>822</v>
+      </c>
+      <c r="C117" t="s">
         <v>823</v>
-      </c>
-      <c r="C117" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -8355,10 +8367,10 @@
         <v>619</v>
       </c>
       <c r="B118" t="s">
+        <v>767</v>
+      </c>
+      <c r="C118" t="s">
         <v>768</v>
-      </c>
-      <c r="C118" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -8366,10 +8378,10 @@
         <v>619</v>
       </c>
       <c r="B119" t="s">
+        <v>769</v>
+      </c>
+      <c r="C119" t="s">
         <v>770</v>
-      </c>
-      <c r="C119" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -8377,10 +8389,10 @@
         <v>619</v>
       </c>
       <c r="B120" t="s">
+        <v>771</v>
+      </c>
+      <c r="C120" t="s">
         <v>772</v>
-      </c>
-      <c r="C120" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -8388,10 +8400,10 @@
         <v>619</v>
       </c>
       <c r="B121" t="s">
+        <v>773</v>
+      </c>
+      <c r="C121" t="s">
         <v>774</v>
-      </c>
-      <c r="C121" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -8399,10 +8411,10 @@
         <v>619</v>
       </c>
       <c r="B122" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C122" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -8413,7 +8425,7 @@
         <v>730</v>
       </c>
       <c r="C123" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -8421,10 +8433,10 @@
         <v>619</v>
       </c>
       <c r="B124" t="s">
+        <v>778</v>
+      </c>
+      <c r="C124" t="s">
         <v>779</v>
-      </c>
-      <c r="C124" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -8432,10 +8444,10 @@
         <v>619</v>
       </c>
       <c r="B125" t="s">
+        <v>780</v>
+      </c>
+      <c r="C125" t="s">
         <v>781</v>
-      </c>
-      <c r="C125" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -8443,10 +8455,10 @@
         <v>619</v>
       </c>
       <c r="B126" t="s">
+        <v>782</v>
+      </c>
+      <c r="C126" t="s">
         <v>783</v>
-      </c>
-      <c r="C126" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -8454,10 +8466,10 @@
         <v>619</v>
       </c>
       <c r="B127" t="s">
+        <v>784</v>
+      </c>
+      <c r="C127" t="s">
         <v>785</v>
-      </c>
-      <c r="C127" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -8465,10 +8477,10 @@
         <v>619</v>
       </c>
       <c r="B128" t="s">
+        <v>786</v>
+      </c>
+      <c r="C128" t="s">
         <v>787</v>
-      </c>
-      <c r="C128" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -8476,10 +8488,10 @@
         <v>619</v>
       </c>
       <c r="B129" t="s">
+        <v>788</v>
+      </c>
+      <c r="C129" t="s">
         <v>789</v>
-      </c>
-      <c r="C129" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -8487,10 +8499,10 @@
         <v>619</v>
       </c>
       <c r="B130" t="s">
+        <v>790</v>
+      </c>
+      <c r="C130" t="s">
         <v>791</v>
-      </c>
-      <c r="C130" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -8498,10 +8510,10 @@
         <v>619</v>
       </c>
       <c r="B131" t="s">
+        <v>792</v>
+      </c>
+      <c r="C131" t="s">
         <v>793</v>
-      </c>
-      <c r="C131" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -8509,10 +8521,10 @@
         <v>619</v>
       </c>
       <c r="B132" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C132" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -8520,10 +8532,10 @@
         <v>619</v>
       </c>
       <c r="B133" t="s">
+        <v>794</v>
+      </c>
+      <c r="C133" t="s">
         <v>795</v>
-      </c>
-      <c r="C133" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -8531,10 +8543,10 @@
         <v>619</v>
       </c>
       <c r="B134" t="s">
+        <v>796</v>
+      </c>
+      <c r="C134" t="s">
         <v>797</v>
-      </c>
-      <c r="C134" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -8542,10 +8554,10 @@
         <v>619</v>
       </c>
       <c r="B135" t="s">
+        <v>798</v>
+      </c>
+      <c r="C135" t="s">
         <v>799</v>
-      </c>
-      <c r="C135" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -8553,10 +8565,10 @@
         <v>619</v>
       </c>
       <c r="B136" t="s">
+        <v>800</v>
+      </c>
+      <c r="C136" t="s">
         <v>801</v>
-      </c>
-      <c r="C136" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -8564,10 +8576,10 @@
         <v>619</v>
       </c>
       <c r="B137" t="s">
+        <v>802</v>
+      </c>
+      <c r="C137" t="s">
         <v>803</v>
-      </c>
-      <c r="C137" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -8575,10 +8587,10 @@
         <v>619</v>
       </c>
       <c r="B138" t="s">
+        <v>804</v>
+      </c>
+      <c r="C138" t="s">
         <v>805</v>
-      </c>
-      <c r="C138" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -8586,10 +8598,10 @@
         <v>619</v>
       </c>
       <c r="B139" t="s">
+        <v>806</v>
+      </c>
+      <c r="C139" t="s">
         <v>807</v>
-      </c>
-      <c r="C139" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -8597,10 +8609,10 @@
         <v>619</v>
       </c>
       <c r="B140" t="s">
+        <v>808</v>
+      </c>
+      <c r="C140" t="s">
         <v>809</v>
-      </c>
-      <c r="C140" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -8608,10 +8620,10 @@
         <v>619</v>
       </c>
       <c r="B141" t="s">
+        <v>810</v>
+      </c>
+      <c r="C141" t="s">
         <v>811</v>
-      </c>
-      <c r="C141" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -8619,10 +8631,10 @@
         <v>619</v>
       </c>
       <c r="B142" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C142" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -8630,10 +8642,10 @@
         <v>619</v>
       </c>
       <c r="B143" t="s">
+        <v>813</v>
+      </c>
+      <c r="C143" t="s">
         <v>814</v>
-      </c>
-      <c r="C143" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -8641,10 +8653,10 @@
         <v>619</v>
       </c>
       <c r="B144" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C144" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -8652,10 +8664,10 @@
         <v>619</v>
       </c>
       <c r="B145" t="s">
+        <v>818</v>
+      </c>
+      <c r="C145" t="s">
         <v>819</v>
-      </c>
-      <c r="C145" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -8663,10 +8675,10 @@
         <v>619</v>
       </c>
       <c r="B146" t="s">
+        <v>820</v>
+      </c>
+      <c r="C146" t="s">
         <v>821</v>
-      </c>
-      <c r="C146" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -8674,10 +8686,10 @@
         <v>619</v>
       </c>
       <c r="B147" t="s">
+        <v>826</v>
+      </c>
+      <c r="C147" t="s">
         <v>827</v>
-      </c>
-      <c r="C147" t="s">
-        <v>828</v>
       </c>
       <c r="F147" s="8"/>
     </row>
@@ -8710,10 +8722,10 @@
         <v>619</v>
       </c>
       <c r="B150" t="s">
-        <v>762</v>
+        <v>831</v>
       </c>
       <c r="C150" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -8721,10 +8733,10 @@
         <v>619</v>
       </c>
       <c r="B151" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C151" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -8735,7 +8747,7 @@
         <v>741</v>
       </c>
       <c r="C152" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -8743,10 +8755,10 @@
         <v>619</v>
       </c>
       <c r="B153" t="s">
+        <v>828</v>
+      </c>
+      <c r="C153" t="s">
         <v>829</v>
-      </c>
-      <c r="C153" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -8754,32 +8766,33 @@
         <v>619</v>
       </c>
       <c r="B154" t="s">
-        <v>624</v>
+        <v>832</v>
       </c>
       <c r="C154" t="s">
-        <v>625</v>
+        <v>833</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B155" t="s">
-        <v>648</v>
+        <v>834</v>
       </c>
       <c r="C155" t="s">
-        <v>649</v>
-      </c>
+        <v>835</v>
+      </c>
+      <c r="E155" s="8"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B156" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="C156" t="s">
-        <v>651</v>
+        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -8787,10 +8800,10 @@
         <v>647</v>
       </c>
       <c r="B157" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C157" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -8798,10 +8811,10 @@
         <v>647</v>
       </c>
       <c r="B158" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C158" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -8809,10 +8822,10 @@
         <v>647</v>
       </c>
       <c r="B159" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C159" t="s">
-        <v>473</v>
+        <v>653</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -8820,10 +8833,10 @@
         <v>647</v>
       </c>
       <c r="B160" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C160" t="s">
-        <v>475</v>
+        <v>655</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -8834,7 +8847,7 @@
         <v>656</v>
       </c>
       <c r="C161" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -8845,7 +8858,7 @@
         <v>656</v>
       </c>
       <c r="C162" t="s">
-        <v>657</v>
+        <v>475</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -8853,10 +8866,10 @@
         <v>647</v>
       </c>
       <c r="B163" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C163" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -8864,10 +8877,10 @@
         <v>647</v>
       </c>
       <c r="B164" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C164" t="s">
-        <v>484</v>
+        <v>657</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -8875,10 +8888,10 @@
         <v>647</v>
       </c>
       <c r="B165" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C165" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -8886,10 +8899,10 @@
         <v>647</v>
       </c>
       <c r="B166" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C166" t="s">
-        <v>662</v>
+        <v>484</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -8897,10 +8910,10 @@
         <v>647</v>
       </c>
       <c r="B167" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C167" t="s">
-        <v>664</v>
+        <v>486</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -8908,10 +8921,10 @@
         <v>647</v>
       </c>
       <c r="B168" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C168" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -8919,10 +8932,10 @@
         <v>647</v>
       </c>
       <c r="B169" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C169" t="s">
-        <v>488</v>
+        <v>664</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -8930,10 +8943,10 @@
         <v>647</v>
       </c>
       <c r="B170" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C170" t="s">
-        <v>492</v>
+        <v>666</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -8941,10 +8954,10 @@
         <v>647</v>
       </c>
       <c r="B171" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C171" t="s">
-        <v>670</v>
+        <v>488</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -8952,10 +8965,10 @@
         <v>647</v>
       </c>
       <c r="B172" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C172" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -8963,10 +8976,10 @@
         <v>647</v>
       </c>
       <c r="B173" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C173" t="s">
-        <v>510</v>
+        <v>670</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -8974,10 +8987,10 @@
         <v>647</v>
       </c>
       <c r="B174" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C174" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -8985,10 +8998,10 @@
         <v>647</v>
       </c>
       <c r="B175" t="s">
-        <v>493</v>
+        <v>672</v>
       </c>
       <c r="C175" t="s">
-        <v>494</v>
+        <v>510</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -8996,10 +9009,10 @@
         <v>647</v>
       </c>
       <c r="B176" t="s">
-        <v>495</v>
+        <v>673</v>
       </c>
       <c r="C176" t="s">
-        <v>496</v>
+        <v>512</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -9007,10 +9020,10 @@
         <v>647</v>
       </c>
       <c r="B177" t="s">
-        <v>674</v>
+        <v>493</v>
       </c>
       <c r="C177" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -9018,10 +9031,10 @@
         <v>647</v>
       </c>
       <c r="B178" t="s">
-        <v>675</v>
+        <v>495</v>
       </c>
       <c r="C178" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -9029,10 +9042,10 @@
         <v>647</v>
       </c>
       <c r="B179" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C179" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -9040,10 +9053,10 @@
         <v>647</v>
       </c>
       <c r="B180" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C180" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -9051,10 +9064,10 @@
         <v>647</v>
       </c>
       <c r="B181" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C181" t="s">
-        <v>679</v>
+        <v>502</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -9062,10 +9075,10 @@
         <v>647</v>
       </c>
       <c r="B182" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="C182" t="s">
-        <v>681</v>
+        <v>504</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -9073,10 +9086,10 @@
         <v>647</v>
       </c>
       <c r="B183" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C183" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -9084,10 +9097,10 @@
         <v>647</v>
       </c>
       <c r="B184" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C184" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -9095,10 +9108,10 @@
         <v>647</v>
       </c>
       <c r="B185" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C185" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -9106,10 +9119,10 @@
         <v>647</v>
       </c>
       <c r="B186" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="C186" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -9117,10 +9130,10 @@
         <v>647</v>
       </c>
       <c r="B187" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C187" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -9128,10 +9141,10 @@
         <v>647</v>
       </c>
       <c r="B188" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="C188" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -9139,10 +9152,10 @@
         <v>647</v>
       </c>
       <c r="B189" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C189" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -9150,10 +9163,10 @@
         <v>647</v>
       </c>
       <c r="B190" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C190" t="s">
-        <v>518</v>
+        <v>693</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -9161,10 +9174,10 @@
         <v>647</v>
       </c>
       <c r="B191" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C191" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -9172,10 +9185,10 @@
         <v>647</v>
       </c>
       <c r="B192" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="C192" t="s">
-        <v>700</v>
+        <v>518</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -9183,10 +9196,10 @@
         <v>647</v>
       </c>
       <c r="B193" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C193" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -9194,10 +9207,10 @@
         <v>647</v>
       </c>
       <c r="B194" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C194" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -9205,10 +9218,10 @@
         <v>647</v>
       </c>
       <c r="B195" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="C195" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -9216,9 +9229,31 @@
         <v>647</v>
       </c>
       <c r="B196" t="s">
+        <v>703</v>
+      </c>
+      <c r="C196" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>647</v>
+      </c>
+      <c r="B197" t="s">
+        <v>708</v>
+      </c>
+      <c r="C197" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>647</v>
+      </c>
+      <c r="B198" t="s">
         <v>706</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C198" t="s">
         <v>707</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Operation Mode BiogasPlant Complete- creation a machine learning model for biogas plant
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\project-cali\backend\v1.0\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C0C144-C7D6-46F1-AF9E-90FE417FA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -2619,7 +2619,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2987,13 +2987,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>275</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>436</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>436</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>519</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>436</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E10" s="8"/>
     </row>
   </sheetData>
@@ -3110,13 +3110,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>275</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>435</v>
       </c>
@@ -3154,17 +3154,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>428</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3395,136 +3395,136 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
     </row>
   </sheetData>
@@ -3540,18 +3540,18 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>211</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>212</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>213</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>214</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>215</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>217</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>218</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>219</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>220</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>223</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>224</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>225</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>226</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>227</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>228</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>230</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>233</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>234</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>235</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>236</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>237</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>238</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>240</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>242</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>243</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>244</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>245</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>246</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>247</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>116</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>118</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>248</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>249</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>250</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>251</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>252</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>253</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>254</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>255</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>256</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>257</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>258</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>259</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>260</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>261</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>262</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>263</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>264</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>265</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>266</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>267</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>268</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>269</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>270</v>
       </c>
@@ -6480,7 +6480,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>271</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>272</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>273</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>60</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>62</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>64</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>66</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>70</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>74</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>76</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>78</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>80</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>82</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>84</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>86</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>88</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>90</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>92</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>94</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>96</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>98</v>
       </c>
@@ -7090,16 +7090,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>465</v>
       </c>
@@ -7110,7 +7112,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -7121,7 +7123,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -7132,7 +7134,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>467</v>
       </c>
@@ -7143,7 +7145,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>467</v>
       </c>
@@ -7154,7 +7156,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>467</v>
       </c>
@@ -7165,7 +7167,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>467</v>
       </c>
@@ -7176,7 +7178,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>467</v>
       </c>
@@ -7187,7 +7189,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -7198,7 +7200,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>467</v>
       </c>
@@ -7209,7 +7211,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>467</v>
       </c>
@@ -7220,7 +7222,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>467</v>
       </c>
@@ -7231,7 +7233,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>467</v>
       </c>
@@ -7242,7 +7244,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>467</v>
       </c>
@@ -7253,7 +7255,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>467</v>
       </c>
@@ -7264,7 +7266,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>467</v>
       </c>
@@ -7275,7 +7277,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>467</v>
       </c>
@@ -7286,7 +7288,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>467</v>
       </c>
@@ -7297,7 +7299,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>467</v>
       </c>
@@ -7308,7 +7310,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>467</v>
       </c>
@@ -7319,7 +7321,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>467</v>
       </c>
@@ -7330,7 +7332,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>467</v>
       </c>
@@ -7341,7 +7343,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>467</v>
       </c>
@@ -7352,7 +7354,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>467</v>
       </c>
@@ -7363,7 +7365,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>467</v>
       </c>
@@ -7374,7 +7376,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>467</v>
       </c>
@@ -7385,7 +7387,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>467</v>
       </c>
@@ -7396,7 +7398,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>467</v>
       </c>
@@ -7407,7 +7409,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>467</v>
       </c>
@@ -7418,7 +7420,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>467</v>
       </c>
@@ -7429,7 +7431,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>467</v>
       </c>
@@ -7440,7 +7442,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>467</v>
       </c>
@@ -7451,7 +7453,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>467</v>
       </c>
@@ -7462,7 +7464,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>467</v>
       </c>
@@ -7473,7 +7475,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>467</v>
       </c>
@@ -7484,7 +7486,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>467</v>
       </c>
@@ -7495,7 +7497,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>522</v>
       </c>
@@ -7506,7 +7508,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>522</v>
       </c>
@@ -7517,7 +7519,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>522</v>
       </c>
@@ -7528,7 +7530,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>522</v>
       </c>
@@ -7539,7 +7541,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>522</v>
       </c>
@@ -7550,7 +7552,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>522</v>
       </c>
@@ -7561,7 +7563,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>522</v>
       </c>
@@ -7572,7 +7574,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>522</v>
       </c>
@@ -7583,7 +7585,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>522</v>
       </c>
@@ -7594,7 +7596,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>522</v>
       </c>
@@ -7605,7 +7607,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>522</v>
       </c>
@@ -7616,7 +7618,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>522</v>
       </c>
@@ -7627,7 +7629,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>522</v>
       </c>
@@ -7638,7 +7640,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>522</v>
       </c>
@@ -7649,7 +7651,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>522</v>
       </c>
@@ -7660,7 +7662,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>522</v>
       </c>
@@ -7671,7 +7673,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>522</v>
       </c>
@@ -7682,7 +7684,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>522</v>
       </c>
@@ -7693,7 +7695,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>522</v>
       </c>
@@ -7704,7 +7706,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>522</v>
       </c>
@@ -7715,7 +7717,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>522</v>
       </c>
@@ -7726,7 +7728,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>522</v>
       </c>
@@ -7737,7 +7739,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>522</v>
       </c>
@@ -7748,7 +7750,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>522</v>
       </c>
@@ -7759,7 +7761,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>522</v>
       </c>
@@ -7770,7 +7772,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>522</v>
       </c>
@@ -7781,7 +7783,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>522</v>
       </c>
@@ -7792,7 +7794,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>522</v>
       </c>
@@ -7803,7 +7805,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>522</v>
       </c>
@@ -7814,7 +7816,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>522</v>
       </c>
@@ -7825,7 +7827,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>522</v>
       </c>
@@ -7836,7 +7838,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>522</v>
       </c>
@@ -7847,7 +7849,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>522</v>
       </c>
@@ -7858,7 +7860,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>522</v>
       </c>
@@ -7869,7 +7871,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>522</v>
       </c>
@@ -7880,7 +7882,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>522</v>
       </c>
@@ -7891,7 +7893,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>522</v>
       </c>
@@ -7902,7 +7904,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>522</v>
       </c>
@@ -7913,7 +7915,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>522</v>
       </c>
@@ -7924,7 +7926,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>522</v>
       </c>
@@ -7935,7 +7937,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>522</v>
       </c>
@@ -7946,7 +7948,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>522</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>522</v>
       </c>
@@ -7968,7 +7970,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>522</v>
       </c>
@@ -7979,7 +7981,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>522</v>
       </c>
@@ -7990,7 +7992,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>522</v>
       </c>
@@ -8001,7 +8003,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>522</v>
       </c>
@@ -8012,7 +8014,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>522</v>
       </c>
@@ -8023,7 +8025,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>522</v>
       </c>
@@ -8034,7 +8036,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>522</v>
       </c>
@@ -8045,7 +8047,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>522</v>
       </c>
@@ -8056,7 +8058,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>522</v>
       </c>
@@ -8067,7 +8069,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>522</v>
       </c>
@@ -8078,7 +8080,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>522</v>
       </c>
@@ -8089,7 +8091,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>522</v>
       </c>
@@ -8100,7 +8102,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>522</v>
       </c>
@@ -8111,7 +8113,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>522</v>
       </c>
@@ -8122,7 +8124,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>522</v>
       </c>
@@ -8133,7 +8135,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>522</v>
       </c>
@@ -8144,7 +8146,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>522</v>
       </c>
@@ -8155,7 +8157,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>522</v>
       </c>
@@ -8166,7 +8168,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>522</v>
       </c>
@@ -8177,7 +8179,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>619</v>
       </c>
@@ -8188,7 +8190,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>619</v>
       </c>
@@ -8199,7 +8201,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>619</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>619</v>
       </c>
@@ -8221,7 +8223,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>619</v>
       </c>
@@ -8232,7 +8234,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>619</v>
       </c>
@@ -8243,7 +8245,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>619</v>
       </c>
@@ -8254,7 +8256,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>619</v>
       </c>
@@ -8265,7 +8267,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>619</v>
       </c>
@@ -8276,7 +8278,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>619</v>
       </c>
@@ -8287,7 +8289,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>619</v>
       </c>
@@ -8298,7 +8300,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>619</v>
       </c>
@@ -8309,7 +8311,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>619</v>
       </c>
@@ -8320,7 +8322,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>619</v>
       </c>
@@ -8331,7 +8333,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>619</v>
       </c>
@@ -8342,7 +8344,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>619</v>
       </c>
@@ -8353,7 +8355,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>619</v>
       </c>
@@ -8364,7 +8366,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>619</v>
       </c>
@@ -8375,7 +8377,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>619</v>
       </c>
@@ -8386,7 +8388,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>619</v>
       </c>
@@ -8397,7 +8399,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>619</v>
       </c>
@@ -8408,7 +8410,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>619</v>
       </c>
@@ -8419,7 +8421,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>619</v>
       </c>
@@ -8430,7 +8432,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>619</v>
       </c>
@@ -8441,7 +8443,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>619</v>
       </c>
@@ -8452,7 +8454,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>619</v>
       </c>
@@ -8463,7 +8465,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>619</v>
       </c>
@@ -8474,7 +8476,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>619</v>
       </c>
@@ -8485,7 +8487,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>619</v>
       </c>
@@ -8496,7 +8498,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>619</v>
       </c>
@@ -8507,7 +8509,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>619</v>
       </c>
@@ -8518,7 +8520,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>619</v>
       </c>
@@ -8529,7 +8531,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>619</v>
       </c>
@@ -8540,7 +8542,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>619</v>
       </c>
@@ -8551,7 +8553,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>619</v>
       </c>
@@ -8562,7 +8564,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>619</v>
       </c>
@@ -8573,7 +8575,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>619</v>
       </c>
@@ -8584,7 +8586,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>619</v>
       </c>
@@ -8595,7 +8597,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>619</v>
       </c>
@@ -8606,7 +8608,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>619</v>
       </c>
@@ -8617,7 +8619,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>619</v>
       </c>
@@ -8628,7 +8630,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>619</v>
       </c>
@@ -8639,7 +8641,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>619</v>
       </c>
@@ -8650,7 +8652,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>619</v>
       </c>
@@ -8661,7 +8663,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>619</v>
       </c>
@@ -8672,7 +8674,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>619</v>
       </c>
@@ -8683,7 +8685,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>619</v>
       </c>
@@ -8694,7 +8696,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>619</v>
       </c>
@@ -8705,7 +8707,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>619</v>
       </c>
@@ -8717,7 +8719,7 @@
       </c>
       <c r="F147" s="8"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>619</v>
       </c>
@@ -8730,7 +8732,7 @@
       <c r="F148" s="8"/>
       <c r="G148" s="8"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>619</v>
       </c>
@@ -8741,7 +8743,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>619</v>
       </c>
@@ -8752,7 +8754,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>619</v>
       </c>
@@ -8763,7 +8765,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>619</v>
       </c>
@@ -8774,7 +8776,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>619</v>
       </c>
@@ -8785,7 +8787,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>619</v>
       </c>
@@ -8796,7 +8798,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>619</v>
       </c>
@@ -8808,7 +8810,7 @@
       </c>
       <c r="E155" s="8"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>619</v>
       </c>
@@ -8819,7 +8821,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>647</v>
       </c>
@@ -8830,7 +8832,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>647</v>
       </c>
@@ -8841,7 +8843,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>647</v>
       </c>
@@ -8852,7 +8854,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>647</v>
       </c>
@@ -8863,7 +8865,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>647</v>
       </c>
@@ -8874,7 +8876,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>647</v>
       </c>
@@ -8885,7 +8887,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>647</v>
       </c>
@@ -8896,7 +8898,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>647</v>
       </c>
@@ -8907,7 +8909,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>647</v>
       </c>
@@ -8918,7 +8920,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>647</v>
       </c>
@@ -8929,7 +8931,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>647</v>
       </c>
@@ -8940,7 +8942,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>647</v>
       </c>
@@ -8951,7 +8953,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>647</v>
       </c>
@@ -8962,7 +8964,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>647</v>
       </c>
@@ -8973,7 +8975,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>647</v>
       </c>
@@ -8984,7 +8986,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>647</v>
       </c>
@@ -8995,7 +8997,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>647</v>
       </c>
@@ -9006,7 +9008,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>647</v>
       </c>
@@ -9017,7 +9019,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>647</v>
       </c>
@@ -9028,7 +9030,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>647</v>
       </c>
@@ -9039,7 +9041,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>647</v>
       </c>
@@ -9050,7 +9052,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>647</v>
       </c>
@@ -9061,7 +9063,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>647</v>
       </c>
@@ -9072,7 +9074,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>647</v>
       </c>
@@ -9083,7 +9085,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>647</v>
       </c>
@@ -9094,7 +9096,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>647</v>
       </c>
@@ -9105,7 +9107,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>647</v>
       </c>
@@ -9116,7 +9118,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>647</v>
       </c>
@@ -9127,7 +9129,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>647</v>
       </c>
@@ -9138,7 +9140,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>647</v>
       </c>
@@ -9149,7 +9151,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>647</v>
       </c>
@@ -9160,7 +9162,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>647</v>
       </c>
@@ -9171,7 +9173,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>647</v>
       </c>
@@ -9182,7 +9184,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>647</v>
       </c>
@@ -9193,7 +9195,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>647</v>
       </c>
@@ -9204,7 +9206,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>647</v>
       </c>
@@ -9215,7 +9217,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>647</v>
       </c>
@@ -9226,7 +9228,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>647</v>
       </c>
@@ -9237,7 +9239,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>647</v>
       </c>
@@ -9248,7 +9250,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>647</v>
       </c>
@@ -9259,7 +9261,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>647</v>
       </c>
@@ -9270,7 +9272,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>647</v>
       </c>
@@ -9281,7 +9283,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>647</v>
       </c>
@@ -9292,7 +9294,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>647</v>
       </c>
@@ -9303,7 +9305,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>647</v>
       </c>
@@ -9314,7 +9316,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>647</v>
       </c>
@@ -9325,7 +9327,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>647</v>
       </c>
@@ -9336,7 +9338,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>647</v>
       </c>
@@ -9347,7 +9349,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>647</v>
       </c>

</xml_diff>

<commit_message>
Update biogas model API
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C0C144-C7D6-46F1-AF9E-90FE417FA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{58C0C144-C7D6-46F1-AF9E-90FE417FA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1540902-0480-4383-9ED3-A9D4D3CE8DCC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="848">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -2613,6 +2613,12 @@
   </si>
   <si>
     <t>VG004</t>
+  </si>
+  <si>
+    <t>Temperatura Mannual R-102</t>
+  </si>
+  <si>
+    <t>TE-102v</t>
   </si>
 </sst>
 </file>
@@ -7088,10 +7094,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:G205"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8228,10 +8234,10 @@
         <v>619</v>
       </c>
       <c r="B103" t="s">
-        <v>711</v>
+        <v>846</v>
       </c>
       <c r="C103" t="s">
-        <v>712</v>
+        <v>847</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -8239,10 +8245,10 @@
         <v>619</v>
       </c>
       <c r="B104" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="C104" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -8250,10 +8256,10 @@
         <v>619</v>
       </c>
       <c r="B105" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C105" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -8261,10 +8267,10 @@
         <v>619</v>
       </c>
       <c r="B106" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C106" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -8272,10 +8278,10 @@
         <v>619</v>
       </c>
       <c r="B107" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C107" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -8283,10 +8289,10 @@
         <v>619</v>
       </c>
       <c r="B108" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C108" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -8294,10 +8300,10 @@
         <v>619</v>
       </c>
       <c r="B109" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C109" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -8305,10 +8311,10 @@
         <v>619</v>
       </c>
       <c r="B110" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C110" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -8316,10 +8322,10 @@
         <v>619</v>
       </c>
       <c r="B111" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C111" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -8327,10 +8333,10 @@
         <v>619</v>
       </c>
       <c r="B112" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C112" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -8338,10 +8344,10 @@
         <v>619</v>
       </c>
       <c r="B113" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C113" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -8349,10 +8355,10 @@
         <v>619</v>
       </c>
       <c r="B114" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C114" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -8360,10 +8366,10 @@
         <v>619</v>
       </c>
       <c r="B115" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C115" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -8371,10 +8377,10 @@
         <v>619</v>
       </c>
       <c r="B116" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C116" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -8382,10 +8388,10 @@
         <v>619</v>
       </c>
       <c r="B117" t="s">
-        <v>820</v>
+        <v>736</v>
       </c>
       <c r="C117" t="s">
-        <v>821</v>
+        <v>738</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -8393,10 +8399,10 @@
         <v>619</v>
       </c>
       <c r="B118" t="s">
-        <v>765</v>
+        <v>820</v>
       </c>
       <c r="C118" t="s">
-        <v>766</v>
+        <v>821</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -8404,10 +8410,10 @@
         <v>619</v>
       </c>
       <c r="B119" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C119" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -8415,10 +8421,10 @@
         <v>619</v>
       </c>
       <c r="B120" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C120" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -8426,10 +8432,10 @@
         <v>619</v>
       </c>
       <c r="B121" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C121" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -8437,10 +8443,10 @@
         <v>619</v>
       </c>
       <c r="B122" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="C122" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -8448,10 +8454,10 @@
         <v>619</v>
       </c>
       <c r="B123" t="s">
-        <v>728</v>
+        <v>774</v>
       </c>
       <c r="C123" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -8459,10 +8465,10 @@
         <v>619</v>
       </c>
       <c r="B124" t="s">
-        <v>776</v>
+        <v>728</v>
       </c>
       <c r="C124" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -8470,10 +8476,10 @@
         <v>619</v>
       </c>
       <c r="B125" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C125" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -8481,10 +8487,10 @@
         <v>619</v>
       </c>
       <c r="B126" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C126" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -8492,10 +8498,10 @@
         <v>619</v>
       </c>
       <c r="B127" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C127" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -8503,10 +8509,10 @@
         <v>619</v>
       </c>
       <c r="B128" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C128" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -8514,10 +8520,10 @@
         <v>619</v>
       </c>
       <c r="B129" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C129" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -8525,10 +8531,10 @@
         <v>619</v>
       </c>
       <c r="B130" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C130" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -8536,10 +8542,10 @@
         <v>619</v>
       </c>
       <c r="B131" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C131" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -8547,10 +8553,10 @@
         <v>619</v>
       </c>
       <c r="B132" t="s">
-        <v>823</v>
+        <v>790</v>
       </c>
       <c r="C132" t="s">
-        <v>822</v>
+        <v>791</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -8558,10 +8564,10 @@
         <v>619</v>
       </c>
       <c r="B133" t="s">
-        <v>792</v>
+        <v>823</v>
       </c>
       <c r="C133" t="s">
-        <v>793</v>
+        <v>822</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -8569,10 +8575,10 @@
         <v>619</v>
       </c>
       <c r="B134" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C134" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -8580,10 +8586,10 @@
         <v>619</v>
       </c>
       <c r="B135" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C135" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -8591,10 +8597,10 @@
         <v>619</v>
       </c>
       <c r="B136" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C136" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -8602,10 +8608,10 @@
         <v>619</v>
       </c>
       <c r="B137" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C137" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -8613,10 +8619,10 @@
         <v>619</v>
       </c>
       <c r="B138" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C138" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -8624,10 +8630,10 @@
         <v>619</v>
       </c>
       <c r="B139" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C139" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -8635,10 +8641,10 @@
         <v>619</v>
       </c>
       <c r="B140" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C140" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -8646,10 +8652,10 @@
         <v>619</v>
       </c>
       <c r="B141" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C141" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -8657,10 +8663,10 @@
         <v>619</v>
       </c>
       <c r="B142" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="C142" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -8668,10 +8674,10 @@
         <v>619</v>
       </c>
       <c r="B143" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="C143" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -8679,10 +8685,10 @@
         <v>619</v>
       </c>
       <c r="B144" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C144" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -8690,10 +8696,10 @@
         <v>619</v>
       </c>
       <c r="B145" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="C145" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -8701,10 +8707,10 @@
         <v>619</v>
       </c>
       <c r="B146" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C146" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -8712,46 +8718,46 @@
         <v>619</v>
       </c>
       <c r="B147" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="C147" t="s">
-        <v>825</v>
-      </c>
-      <c r="F147" s="8"/>
+        <v>819</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>619</v>
       </c>
       <c r="B148" t="s">
-        <v>739</v>
+        <v>824</v>
       </c>
       <c r="C148" t="s">
-        <v>740</v>
+        <v>825</v>
       </c>
       <c r="F148" s="8"/>
-      <c r="G148" s="8"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>619</v>
       </c>
       <c r="B149" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="C149" t="s">
-        <v>741</v>
-      </c>
+        <v>740</v>
+      </c>
+      <c r="F149" s="8"/>
+      <c r="G149" s="8"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>619</v>
       </c>
       <c r="B150" t="s">
-        <v>829</v>
+        <v>742</v>
       </c>
       <c r="C150" t="s">
-        <v>763</v>
+        <v>741</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -8759,10 +8765,10 @@
         <v>619</v>
       </c>
       <c r="B151" t="s">
-        <v>760</v>
+        <v>829</v>
       </c>
       <c r="C151" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -8770,10 +8776,10 @@
         <v>619</v>
       </c>
       <c r="B152" t="s">
-        <v>739</v>
+        <v>760</v>
       </c>
       <c r="C152" t="s">
-        <v>828</v>
+        <v>764</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -8781,10 +8787,10 @@
         <v>619</v>
       </c>
       <c r="B153" t="s">
-        <v>826</v>
+        <v>739</v>
       </c>
       <c r="C153" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -8792,10 +8798,10 @@
         <v>619</v>
       </c>
       <c r="B154" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="C154" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -8803,33 +8809,33 @@
         <v>619</v>
       </c>
       <c r="B155" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C155" t="s">
-        <v>833</v>
-      </c>
-      <c r="E155" s="8"/>
+        <v>831</v>
+      </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>619</v>
       </c>
       <c r="B156" t="s">
-        <v>624</v>
+        <v>832</v>
       </c>
       <c r="C156" t="s">
-        <v>625</v>
-      </c>
+        <v>833</v>
+      </c>
+      <c r="E156" s="8"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B157" t="s">
-        <v>648</v>
+        <v>624</v>
       </c>
       <c r="C157" t="s">
-        <v>649</v>
+        <v>625</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -8837,10 +8843,10 @@
         <v>647</v>
       </c>
       <c r="B158" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C158" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -8848,10 +8854,10 @@
         <v>647</v>
       </c>
       <c r="B159" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C159" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -8859,10 +8865,10 @@
         <v>647</v>
       </c>
       <c r="B160" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C160" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -8870,10 +8876,10 @@
         <v>647</v>
       </c>
       <c r="B161" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C161" t="s">
-        <v>473</v>
+        <v>655</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -8884,7 +8890,7 @@
         <v>656</v>
       </c>
       <c r="C162" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -8895,7 +8901,7 @@
         <v>656</v>
       </c>
       <c r="C163" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -8906,7 +8912,7 @@
         <v>656</v>
       </c>
       <c r="C164" t="s">
-        <v>657</v>
+        <v>490</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -8914,10 +8920,10 @@
         <v>647</v>
       </c>
       <c r="B165" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C165" t="s">
-        <v>482</v>
+        <v>657</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -8925,10 +8931,10 @@
         <v>647</v>
       </c>
       <c r="B166" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C166" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -8936,10 +8942,10 @@
         <v>647</v>
       </c>
       <c r="B167" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C167" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -8947,10 +8953,10 @@
         <v>647</v>
       </c>
       <c r="B168" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C168" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -8958,10 +8964,10 @@
         <v>647</v>
       </c>
       <c r="B169" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C169" t="s">
-        <v>663</v>
+        <v>483</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -8969,10 +8975,10 @@
         <v>647</v>
       </c>
       <c r="B170" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C170" t="s">
-        <v>487</v>
+        <v>663</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -8980,10 +8986,10 @@
         <v>647</v>
       </c>
       <c r="B171" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C171" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -8991,10 +8997,10 @@
         <v>647</v>
       </c>
       <c r="B172" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C172" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -9002,10 +9008,10 @@
         <v>647</v>
       </c>
       <c r="B173" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C173" t="s">
-        <v>668</v>
+        <v>492</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -9013,10 +9019,10 @@
         <v>647</v>
       </c>
       <c r="B174" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C174" t="s">
-        <v>508</v>
+        <v>668</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -9024,10 +9030,10 @@
         <v>647</v>
       </c>
       <c r="B175" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C175" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -9035,10 +9041,10 @@
         <v>647</v>
       </c>
       <c r="B176" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C176" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -9046,10 +9052,10 @@
         <v>647</v>
       </c>
       <c r="B177" t="s">
-        <v>493</v>
+        <v>671</v>
       </c>
       <c r="C177" t="s">
-        <v>494</v>
+        <v>512</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -9057,10 +9063,10 @@
         <v>647</v>
       </c>
       <c r="B178" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C178" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -9068,10 +9074,10 @@
         <v>647</v>
       </c>
       <c r="B179" t="s">
-        <v>672</v>
+        <v>495</v>
       </c>
       <c r="C179" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -9079,10 +9085,10 @@
         <v>647</v>
       </c>
       <c r="B180" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C180" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -9090,10 +9096,10 @@
         <v>647</v>
       </c>
       <c r="B181" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C181" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -9101,10 +9107,10 @@
         <v>647</v>
       </c>
       <c r="B182" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C182" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -9112,10 +9118,10 @@
         <v>647</v>
       </c>
       <c r="B183" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C183" t="s">
-        <v>677</v>
+        <v>504</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -9123,10 +9129,10 @@
         <v>647</v>
       </c>
       <c r="B184" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C184" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -9134,10 +9140,10 @@
         <v>647</v>
       </c>
       <c r="B185" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C185" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -9145,10 +9151,10 @@
         <v>647</v>
       </c>
       <c r="B186" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C186" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -9156,10 +9162,10 @@
         <v>647</v>
       </c>
       <c r="B187" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C187" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -9167,10 +9173,10 @@
         <v>647</v>
       </c>
       <c r="B188" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C188" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -9178,10 +9184,10 @@
         <v>647</v>
       </c>
       <c r="B189" t="s">
-        <v>834</v>
+        <v>686</v>
       </c>
       <c r="C189" t="s">
-        <v>754</v>
+        <v>687</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -9189,10 +9195,10 @@
         <v>647</v>
       </c>
       <c r="B190" t="s">
-        <v>688</v>
+        <v>834</v>
       </c>
       <c r="C190" t="s">
-        <v>689</v>
+        <v>754</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -9200,10 +9206,10 @@
         <v>647</v>
       </c>
       <c r="B191" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C191" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -9211,10 +9217,10 @@
         <v>647</v>
       </c>
       <c r="B192" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C192" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -9222,10 +9228,10 @@
         <v>647</v>
       </c>
       <c r="B193" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C193" t="s">
-        <v>518</v>
+        <v>693</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -9233,10 +9239,10 @@
         <v>647</v>
       </c>
       <c r="B194" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C194" t="s">
-        <v>696</v>
+        <v>518</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -9244,10 +9250,10 @@
         <v>647</v>
       </c>
       <c r="B195" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C195" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -9255,10 +9261,10 @@
         <v>647</v>
       </c>
       <c r="B196" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C196" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -9266,10 +9272,10 @@
         <v>647</v>
       </c>
       <c r="B197" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C197" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -9277,10 +9283,10 @@
         <v>647</v>
       </c>
       <c r="B198" t="s">
-        <v>835</v>
+        <v>701</v>
       </c>
       <c r="C198" t="s">
-        <v>836</v>
+        <v>702</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -9288,10 +9294,10 @@
         <v>647</v>
       </c>
       <c r="B199" t="s">
-        <v>706</v>
+        <v>835</v>
       </c>
       <c r="C199" t="s">
-        <v>703</v>
+        <v>836</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -9299,10 +9305,10 @@
         <v>647</v>
       </c>
       <c r="B200" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C200" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -9310,10 +9316,10 @@
         <v>647</v>
       </c>
       <c r="B201" t="s">
-        <v>837</v>
+        <v>704</v>
       </c>
       <c r="C201" t="s">
-        <v>838</v>
+        <v>705</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -9321,10 +9327,10 @@
         <v>647</v>
       </c>
       <c r="B202" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C202" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -9332,10 +9338,10 @@
         <v>647</v>
       </c>
       <c r="B203" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C203" t="s">
-        <v>758</v>
+        <v>840</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
@@ -9343,10 +9349,10 @@
         <v>647</v>
       </c>
       <c r="B204" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C204" t="s">
-        <v>843</v>
+        <v>758</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
@@ -9354,9 +9360,20 @@
         <v>647</v>
       </c>
       <c r="B205" t="s">
+        <v>842</v>
+      </c>
+      <c r="C205" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>647</v>
+      </c>
+      <c r="B206" t="s">
         <v>844</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C206" t="s">
         <v>845</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 2 Machine learning modulo for biogas plant
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sarango_uco_edu_co/Documents/Documents/GitHub/project-cali/backend/v1.0/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{58C0C144-C7D6-46F1-AF9E-90FE417FA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1540902-0480-4383-9ED3-A9D4D3CE8DCC}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{58C0C144-C7D6-46F1-AF9E-90FE417FA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26D596EC-61E0-4018-85FD-A3240495D6C3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1949,12 +1949,6 @@
     <t>TE-101v</t>
   </si>
   <si>
-    <t>K_mean</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>UCO</t>
   </si>
   <si>
@@ -2619,6 +2613,12 @@
   </si>
   <si>
     <t>TE-102v</t>
+  </si>
+  <si>
+    <t>Kinetic_train</t>
+  </si>
+  <si>
+    <t>K_train</t>
   </si>
 </sst>
 </file>
@@ -3097,7 +3097,7 @@
         <v>440</v>
       </c>
       <c r="E5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F5" t="s">
         <v>521</v>
@@ -7100,8 +7100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
   <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7204,7 +7204,7 @@
         <v>467</v>
       </c>
       <c r="B9" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C9" t="s">
         <v>482</v>
@@ -7215,7 +7215,7 @@
         <v>467</v>
       </c>
       <c r="B10" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C10" t="s">
         <v>483</v>
@@ -7226,7 +7226,7 @@
         <v>467</v>
       </c>
       <c r="B11" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C11" t="s">
         <v>484</v>
@@ -7237,7 +7237,7 @@
         <v>467</v>
       </c>
       <c r="B12" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C12" t="s">
         <v>485</v>
@@ -7248,7 +7248,7 @@
         <v>467</v>
       </c>
       <c r="B13" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C13" t="s">
         <v>486</v>
@@ -7259,7 +7259,7 @@
         <v>467</v>
       </c>
       <c r="B14" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C14" t="s">
         <v>487</v>
@@ -7270,7 +7270,7 @@
         <v>467</v>
       </c>
       <c r="B15" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C15" t="s">
         <v>488</v>
@@ -7281,7 +7281,7 @@
         <v>467</v>
       </c>
       <c r="B16" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C16" t="s">
         <v>489</v>
@@ -7292,10 +7292,10 @@
         <v>467</v>
       </c>
       <c r="B17" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C17" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -7303,7 +7303,7 @@
         <v>467</v>
       </c>
       <c r="B18" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C18" t="s">
         <v>490</v>
@@ -7314,10 +7314,10 @@
         <v>467</v>
       </c>
       <c r="B19" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C19" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -7325,10 +7325,10 @@
         <v>467</v>
       </c>
       <c r="B20" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C20" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -7336,10 +7336,10 @@
         <v>467</v>
       </c>
       <c r="B21" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C21" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -7347,10 +7347,10 @@
         <v>467</v>
       </c>
       <c r="B22" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C22" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -7886,10 +7886,10 @@
         <v>522</v>
       </c>
       <c r="B71" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C71" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -8062,10 +8062,10 @@
         <v>522</v>
       </c>
       <c r="B87" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C87" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -8073,10 +8073,10 @@
         <v>522</v>
       </c>
       <c r="B88" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C88" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -8084,7 +8084,7 @@
         <v>522</v>
       </c>
       <c r="B89" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C89" t="s">
         <v>568</v>
@@ -8095,10 +8095,10 @@
         <v>522</v>
       </c>
       <c r="B90" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C90" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -8106,10 +8106,10 @@
         <v>522</v>
       </c>
       <c r="B91" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C91" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -8117,10 +8117,10 @@
         <v>522</v>
       </c>
       <c r="B92" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C92" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -8139,10 +8139,10 @@
         <v>522</v>
       </c>
       <c r="B94" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C94" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -8150,10 +8150,10 @@
         <v>522</v>
       </c>
       <c r="B95" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C95" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -8161,10 +8161,10 @@
         <v>522</v>
       </c>
       <c r="B96" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C96" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -8172,10 +8172,10 @@
         <v>522</v>
       </c>
       <c r="B97" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C97" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -8183,10 +8183,10 @@
         <v>522</v>
       </c>
       <c r="B98" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C98" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -8205,10 +8205,10 @@
         <v>619</v>
       </c>
       <c r="B100" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C100" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -8216,10 +8216,10 @@
         <v>619</v>
       </c>
       <c r="B101" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C101" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -8238,10 +8238,10 @@
         <v>619</v>
       </c>
       <c r="B103" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C103" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -8249,10 +8249,10 @@
         <v>619</v>
       </c>
       <c r="B104" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C104" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -8260,10 +8260,10 @@
         <v>619</v>
       </c>
       <c r="B105" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C105" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -8271,10 +8271,10 @@
         <v>619</v>
       </c>
       <c r="B106" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C106" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -8282,10 +8282,10 @@
         <v>619</v>
       </c>
       <c r="B107" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C107" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -8293,10 +8293,10 @@
         <v>619</v>
       </c>
       <c r="B108" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C108" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -8304,10 +8304,10 @@
         <v>619</v>
       </c>
       <c r="B109" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C109" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -8315,10 +8315,10 @@
         <v>619</v>
       </c>
       <c r="B110" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C110" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -8326,10 +8326,10 @@
         <v>619</v>
       </c>
       <c r="B111" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C111" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -8337,10 +8337,10 @@
         <v>619</v>
       </c>
       <c r="B112" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C112" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -8348,10 +8348,10 @@
         <v>619</v>
       </c>
       <c r="B113" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C113" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -8359,10 +8359,10 @@
         <v>619</v>
       </c>
       <c r="B114" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C114" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -8370,10 +8370,10 @@
         <v>619</v>
       </c>
       <c r="B115" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C115" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -8381,10 +8381,10 @@
         <v>619</v>
       </c>
       <c r="B116" t="s">
+        <v>733</v>
+      </c>
+      <c r="C116" t="s">
         <v>735</v>
-      </c>
-      <c r="C116" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -8392,10 +8392,10 @@
         <v>619</v>
       </c>
       <c r="B117" t="s">
+        <v>734</v>
+      </c>
+      <c r="C117" t="s">
         <v>736</v>
-      </c>
-      <c r="C117" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -8403,10 +8403,10 @@
         <v>619</v>
       </c>
       <c r="B118" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C118" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -8414,10 +8414,10 @@
         <v>619</v>
       </c>
       <c r="B119" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C119" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -8425,10 +8425,10 @@
         <v>619</v>
       </c>
       <c r="B120" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C120" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -8436,10 +8436,10 @@
         <v>619</v>
       </c>
       <c r="B121" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C121" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -8447,10 +8447,10 @@
         <v>619</v>
       </c>
       <c r="B122" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C122" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -8458,10 +8458,10 @@
         <v>619</v>
       </c>
       <c r="B123" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C123" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -8469,10 +8469,10 @@
         <v>619</v>
       </c>
       <c r="B124" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C124" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -8480,10 +8480,10 @@
         <v>619</v>
       </c>
       <c r="B125" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C125" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -8491,10 +8491,10 @@
         <v>619</v>
       </c>
       <c r="B126" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C126" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -8502,10 +8502,10 @@
         <v>619</v>
       </c>
       <c r="B127" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C127" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -8513,10 +8513,10 @@
         <v>619</v>
       </c>
       <c r="B128" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C128" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -8524,10 +8524,10 @@
         <v>619</v>
       </c>
       <c r="B129" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C129" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -8535,10 +8535,10 @@
         <v>619</v>
       </c>
       <c r="B130" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C130" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -8546,10 +8546,10 @@
         <v>619</v>
       </c>
       <c r="B131" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C131" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -8557,10 +8557,10 @@
         <v>619</v>
       </c>
       <c r="B132" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C132" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -8568,10 +8568,10 @@
         <v>619</v>
       </c>
       <c r="B133" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C133" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -8579,10 +8579,10 @@
         <v>619</v>
       </c>
       <c r="B134" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C134" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -8590,10 +8590,10 @@
         <v>619</v>
       </c>
       <c r="B135" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C135" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -8601,10 +8601,10 @@
         <v>619</v>
       </c>
       <c r="B136" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C136" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -8612,10 +8612,10 @@
         <v>619</v>
       </c>
       <c r="B137" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C137" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -8623,10 +8623,10 @@
         <v>619</v>
       </c>
       <c r="B138" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C138" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -8634,10 +8634,10 @@
         <v>619</v>
       </c>
       <c r="B139" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C139" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -8645,10 +8645,10 @@
         <v>619</v>
       </c>
       <c r="B140" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C140" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -8656,10 +8656,10 @@
         <v>619</v>
       </c>
       <c r="B141" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C141" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -8667,10 +8667,10 @@
         <v>619</v>
       </c>
       <c r="B142" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C142" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -8678,10 +8678,10 @@
         <v>619</v>
       </c>
       <c r="B143" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C143" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -8689,10 +8689,10 @@
         <v>619</v>
       </c>
       <c r="B144" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C144" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -8700,10 +8700,10 @@
         <v>619</v>
       </c>
       <c r="B145" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C145" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -8711,10 +8711,10 @@
         <v>619</v>
       </c>
       <c r="B146" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C146" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -8722,10 +8722,10 @@
         <v>619</v>
       </c>
       <c r="B147" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C147" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -8733,10 +8733,10 @@
         <v>619</v>
       </c>
       <c r="B148" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C148" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F148" s="8"/>
     </row>
@@ -8745,10 +8745,10 @@
         <v>619</v>
       </c>
       <c r="B149" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C149" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F149" s="8"/>
       <c r="G149" s="8"/>
@@ -8758,10 +8758,10 @@
         <v>619</v>
       </c>
       <c r="B150" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C150" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -8769,10 +8769,10 @@
         <v>619</v>
       </c>
       <c r="B151" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C151" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -8780,10 +8780,10 @@
         <v>619</v>
       </c>
       <c r="B152" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C152" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -8791,10 +8791,10 @@
         <v>619</v>
       </c>
       <c r="B153" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C153" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -8802,10 +8802,10 @@
         <v>619</v>
       </c>
       <c r="B154" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C154" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -8813,10 +8813,10 @@
         <v>619</v>
       </c>
       <c r="B155" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C155" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -8824,10 +8824,10 @@
         <v>619</v>
       </c>
       <c r="B156" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C156" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="E156" s="8"/>
     </row>
@@ -8836,62 +8836,62 @@
         <v>619</v>
       </c>
       <c r="B157" t="s">
-        <v>624</v>
+        <v>846</v>
       </c>
       <c r="C157" t="s">
-        <v>625</v>
+        <v>847</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>645</v>
+      </c>
+      <c r="B158" t="s">
+        <v>646</v>
+      </c>
+      <c r="C158" t="s">
         <v>647</v>
-      </c>
-      <c r="B158" t="s">
-        <v>648</v>
-      </c>
-      <c r="C158" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B159" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C159" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B160" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C160" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B161" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C161" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B162" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C162" t="s">
         <v>473</v>
@@ -8899,10 +8899,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B163" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C163" t="s">
         <v>475</v>
@@ -8910,10 +8910,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B164" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C164" t="s">
         <v>490</v>
@@ -8921,21 +8921,21 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B165" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C165" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B166" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C166" t="s">
         <v>482</v>
@@ -8943,10 +8943,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B167" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C167" t="s">
         <v>484</v>
@@ -8954,10 +8954,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B168" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C168" t="s">
         <v>486</v>
@@ -8965,10 +8965,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B169" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C169" t="s">
         <v>483</v>
@@ -8976,21 +8976,21 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B170" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C170" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B171" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C171" t="s">
         <v>487</v>
@@ -8998,10 +8998,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B172" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C172" t="s">
         <v>488</v>
@@ -9009,10 +9009,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B173" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C173" t="s">
         <v>492</v>
@@ -9020,21 +9020,21 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B174" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C174" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B175" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C175" t="s">
         <v>508</v>
@@ -9042,10 +9042,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B176" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C176" t="s">
         <v>510</v>
@@ -9053,10 +9053,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B177" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C177" t="s">
         <v>512</v>
@@ -9064,7 +9064,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B178" t="s">
         <v>493</v>
@@ -9075,7 +9075,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B179" t="s">
         <v>495</v>
@@ -9086,10 +9086,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B180" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C180" t="s">
         <v>498</v>
@@ -9097,10 +9097,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B181" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C181" t="s">
         <v>500</v>
@@ -9108,10 +9108,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B182" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C182" t="s">
         <v>502</v>
@@ -9119,10 +9119,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B183" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C183" t="s">
         <v>504</v>
@@ -9130,120 +9130,120 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B184" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C184" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B185" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C185" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B186" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C186" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B187" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C187" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B188" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C188" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B189" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C189" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B190" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C190" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B191" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C191" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B192" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C192" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B193" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C193" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B194" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C194" t="s">
         <v>518</v>
@@ -9251,134 +9251,134 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B195" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C195" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B196" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C196" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B197" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C197" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B198" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C198" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B199" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C199" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B200" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C200" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B201" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C201" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B202" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C202" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B203" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C203" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B204" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C204" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B205" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C205" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B206" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C206" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Train Model for operation 1
Falta el módulo de pronóstico para el modo de operación 1
</commit_message>
<xml_diff>
--- a/backend/v1.0/tools/DB_Mapping.xlsx
+++ b/backend/v1.0/tools/DB_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarango\OneDrive - UCO\Documents\GitHub\project-cali\backend\v1.0\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\OneDrive - UCO\Documents\GitHub\project-cali\backend\v1.0\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A56CC5-FF53-4F0C-871B-5E2355D253CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEE4277-818B-466A-967B-BA579A5BC3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="849">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -2619,6 +2619,9 @@
   </si>
   <si>
     <t>Temperatura Manual R-102</t>
+  </si>
+  <si>
+    <t>Ea_train</t>
   </si>
 </sst>
 </file>
@@ -7094,10 +7097,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5969C-509B-4D3C-BD42-B92347445C5B}">
-  <dimension ref="A1:G206"/>
+  <dimension ref="A1:G207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8840,13 +8843,13 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>645</v>
+        <v>619</v>
       </c>
       <c r="B158" t="s">
-        <v>646</v>
+        <v>848</v>
       </c>
       <c r="C158" t="s">
-        <v>647</v>
+        <v>848</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -8854,10 +8857,10 @@
         <v>645</v>
       </c>
       <c r="B159" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C159" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -8865,10 +8868,10 @@
         <v>645</v>
       </c>
       <c r="B160" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C160" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -8876,10 +8879,10 @@
         <v>645</v>
       </c>
       <c r="B161" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C161" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -8887,10 +8890,10 @@
         <v>645</v>
       </c>
       <c r="B162" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C162" t="s">
-        <v>473</v>
+        <v>653</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -8901,7 +8904,7 @@
         <v>654</v>
       </c>
       <c r="C163" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -8912,7 +8915,7 @@
         <v>654</v>
       </c>
       <c r="C164" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -8923,7 +8926,7 @@
         <v>654</v>
       </c>
       <c r="C165" t="s">
-        <v>655</v>
+        <v>490</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -8931,10 +8934,10 @@
         <v>645</v>
       </c>
       <c r="B166" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C166" t="s">
-        <v>482</v>
+        <v>655</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -8942,10 +8945,10 @@
         <v>645</v>
       </c>
       <c r="B167" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C167" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -8953,10 +8956,10 @@
         <v>645</v>
       </c>
       <c r="B168" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C168" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -8964,10 +8967,10 @@
         <v>645</v>
       </c>
       <c r="B169" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C169" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -8975,10 +8978,10 @@
         <v>645</v>
       </c>
       <c r="B170" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C170" t="s">
-        <v>661</v>
+        <v>483</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -8986,10 +8989,10 @@
         <v>645</v>
       </c>
       <c r="B171" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C171" t="s">
-        <v>487</v>
+        <v>661</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -8997,10 +9000,10 @@
         <v>645</v>
       </c>
       <c r="B172" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C172" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -9008,10 +9011,10 @@
         <v>645</v>
       </c>
       <c r="B173" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C173" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -9019,10 +9022,10 @@
         <v>645</v>
       </c>
       <c r="B174" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C174" t="s">
-        <v>666</v>
+        <v>492</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -9030,10 +9033,10 @@
         <v>645</v>
       </c>
       <c r="B175" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C175" t="s">
-        <v>508</v>
+        <v>666</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -9041,10 +9044,10 @@
         <v>645</v>
       </c>
       <c r="B176" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C176" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -9052,10 +9055,10 @@
         <v>645</v>
       </c>
       <c r="B177" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C177" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -9063,10 +9066,10 @@
         <v>645</v>
       </c>
       <c r="B178" t="s">
-        <v>493</v>
+        <v>669</v>
       </c>
       <c r="C178" t="s">
-        <v>494</v>
+        <v>512</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -9074,10 +9077,10 @@
         <v>645</v>
       </c>
       <c r="B179" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C179" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -9085,10 +9088,10 @@
         <v>645</v>
       </c>
       <c r="B180" t="s">
-        <v>670</v>
+        <v>495</v>
       </c>
       <c r="C180" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -9096,10 +9099,10 @@
         <v>645</v>
       </c>
       <c r="B181" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C181" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -9107,10 +9110,10 @@
         <v>645</v>
       </c>
       <c r="B182" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C182" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -9118,10 +9121,10 @@
         <v>645</v>
       </c>
       <c r="B183" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C183" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -9129,10 +9132,10 @@
         <v>645</v>
       </c>
       <c r="B184" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C184" t="s">
-        <v>675</v>
+        <v>504</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -9140,10 +9143,10 @@
         <v>645</v>
       </c>
       <c r="B185" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C185" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -9151,10 +9154,10 @@
         <v>645</v>
       </c>
       <c r="B186" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C186" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -9162,10 +9165,10 @@
         <v>645</v>
       </c>
       <c r="B187" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C187" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -9173,10 +9176,10 @@
         <v>645</v>
       </c>
       <c r="B188" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C188" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -9184,10 +9187,10 @@
         <v>645</v>
       </c>
       <c r="B189" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C189" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -9195,10 +9198,10 @@
         <v>645</v>
       </c>
       <c r="B190" t="s">
-        <v>832</v>
+        <v>684</v>
       </c>
       <c r="C190" t="s">
-        <v>752</v>
+        <v>685</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -9206,10 +9209,10 @@
         <v>645</v>
       </c>
       <c r="B191" t="s">
-        <v>686</v>
+        <v>832</v>
       </c>
       <c r="C191" t="s">
-        <v>687</v>
+        <v>752</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -9217,10 +9220,10 @@
         <v>645</v>
       </c>
       <c r="B192" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C192" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -9228,10 +9231,10 @@
         <v>645</v>
       </c>
       <c r="B193" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C193" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -9239,10 +9242,10 @@
         <v>645</v>
       </c>
       <c r="B194" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C194" t="s">
-        <v>518</v>
+        <v>691</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -9250,10 +9253,10 @@
         <v>645</v>
       </c>
       <c r="B195" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C195" t="s">
-        <v>694</v>
+        <v>518</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -9261,10 +9264,10 @@
         <v>645</v>
       </c>
       <c r="B196" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C196" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -9272,10 +9275,10 @@
         <v>645</v>
       </c>
       <c r="B197" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C197" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -9283,10 +9286,10 @@
         <v>645</v>
       </c>
       <c r="B198" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C198" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -9294,10 +9297,10 @@
         <v>645</v>
       </c>
       <c r="B199" t="s">
-        <v>833</v>
+        <v>699</v>
       </c>
       <c r="C199" t="s">
-        <v>834</v>
+        <v>700</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -9305,10 +9308,10 @@
         <v>645</v>
       </c>
       <c r="B200" t="s">
-        <v>704</v>
+        <v>833</v>
       </c>
       <c r="C200" t="s">
-        <v>701</v>
+        <v>834</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -9316,10 +9319,10 @@
         <v>645</v>
       </c>
       <c r="B201" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="C201" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -9327,10 +9330,10 @@
         <v>645</v>
       </c>
       <c r="B202" t="s">
-        <v>835</v>
+        <v>702</v>
       </c>
       <c r="C202" t="s">
-        <v>836</v>
+        <v>703</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -9338,10 +9341,10 @@
         <v>645</v>
       </c>
       <c r="B203" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C203" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
@@ -9349,10 +9352,10 @@
         <v>645</v>
       </c>
       <c r="B204" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C204" t="s">
-        <v>756</v>
+        <v>838</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
@@ -9360,10 +9363,10 @@
         <v>645</v>
       </c>
       <c r="B205" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C205" t="s">
-        <v>841</v>
+        <v>756</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
@@ -9371,9 +9374,20 @@
         <v>645</v>
       </c>
       <c r="B206" t="s">
+        <v>840</v>
+      </c>
+      <c r="C206" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>645</v>
+      </c>
+      <c r="B207" t="s">
         <v>842</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C207" t="s">
         <v>843</v>
       </c>
     </row>

</xml_diff>